<commit_message>
Set maximum annuitization to 80% + QLAC. Reduce annuity and max spend for survivor in both Set-spending and Excel double-checker.
</commit_message>
<xml_diff>
--- a/Check Set-spending Cotton Retirement Plan R Model.xlsx
+++ b/Check Set-spending Cotton Retirement Plan R Model.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>scenario</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>Portfolio Spend</t>
-  </si>
-  <si>
-    <t>DC Age</t>
   </si>
   <si>
     <t>VC Age</t>
@@ -467,7 +464,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -517,7 +514,6 @@
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="258">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1108,8 +1104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1133,16 +1129,16 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>300</v>
+        <v>41</v>
       </c>
       <c r="D1" s="6"/>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2">
-        <v>67</v>
+        <v>80</v>
       </c>
       <c r="D2" s="6"/>
       <c r="K2" s="1"/>
@@ -1153,7 +1149,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D3" s="6"/>
     </row>
@@ -1162,7 +1158,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>0.6</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -1171,7 +1167,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>4.4999999999999998E-2</v>
+        <v>0.04</v>
       </c>
       <c r="D5" s="6"/>
     </row>
@@ -1180,7 +1176,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="6"/>
     </row>
@@ -1189,7 +1185,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.112163431808846</v>
+        <v>0.13494295016855501</v>
       </c>
       <c r="D7" s="6"/>
     </row>
@@ -1198,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.16200000000000001</v>
+        <v>9.9400000000000002E-2</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -1206,8 +1202,8 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
-        <v>50000</v>
+      <c r="B9" s="23">
+        <v>100000</v>
       </c>
       <c r="D9" s="6"/>
     </row>
@@ -1216,7 +1212,7 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -1226,7 +1222,7 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>24540</v>
+        <v>28200</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1246,14 +1242,14 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>29952</v>
+        <v>34416</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>0.05</v>
@@ -1261,7 +1257,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15">
         <v>0.05</v>
@@ -1269,7 +1265,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16">
         <v>2.5000000000000001E-2</v>
@@ -1277,47 +1273,46 @@
     </row>
     <row r="17" spans="1:19">
       <c r="A17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17">
-        <v>45</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:19">
       <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" s="23">
-        <v>4000000</v>
-      </c>
-      <c r="C18" s="8"/>
+        <v>32</v>
+      </c>
+      <c r="B18">
+        <v>65</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F18" s="3">
         <v>33521</v>
       </c>
     </row>
     <row r="19" spans="1:19">
       <c r="A19" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" s="23">
-        <v>200000</v>
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>1617017.3284936899</v>
       </c>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:19">
-      <c r="A20" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+      <c r="B20" s="23">
+        <v>4000000</v>
       </c>
     </row>
     <row r="21" spans="1:19">
       <c r="A21" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="27">
-        <v>4671282.63035898</v>
+        <v>31</v>
+      </c>
+      <c r="B21" s="23">
+        <v>200000</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>14</v>
@@ -1327,27 +1322,27 @@
       <c r="A22" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22" s="11" t="s">
         <v>17</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>18</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="13">
         <f>$B$18-$B$9-($B$6*($B$18-$B$9))</f>
-        <v>1975000</v>
+        <v>0</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G22" s="10" t="s">
-        <v>31</v>
-      </c>
       <c r="H22" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I22" s="10" t="s">
         <v>7</v>
@@ -1359,56 +1354,56 @@
         <v>16</v>
       </c>
       <c r="L22" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="M22" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N22" s="14"/>
       <c r="O22" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:19">
       <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B23" s="2">
-        <v>65</v>
+      <c r="B23" t="b">
+        <v>0</v>
       </c>
       <c r="C23" s="2">
         <v>67</v>
       </c>
       <c r="D23">
-        <v>0.123108782674708</v>
+        <v>0.12642260094406699</v>
       </c>
       <c r="E23" s="3">
         <f t="shared" ref="E23:E62" si="0">(E22-K23+MAX(0,M23))*(1+D23)</f>
-        <v>2131986.1710635712</v>
+        <v>0</v>
       </c>
       <c r="F23" s="3">
         <f>IF(C23&gt;=$B$10,$B$11*(1+$B$16)^(A23-1),0)</f>
-        <v>24540</v>
+        <v>0</v>
       </c>
       <c r="G23" s="3">
         <f t="shared" ref="G23:G62" si="1">IF(B23&gt;=$B$12,$B$13*(1+$B$16)^(A23-1),0)</f>
-        <v>0</v>
+        <v>34416</v>
       </c>
       <c r="H23" s="3">
         <f t="shared" ref="H23:H29" si="2">IF(AND(B23&lt;&gt;" ",C23&lt;&gt;" "),F23+G23,IF(AND(B23=" ",C23=" ")," ",MAX(F23,G23)))</f>
-        <v>24540</v>
+        <v>34416</v>
       </c>
       <c r="J23" s="4">
         <f>$B$6*($B$18-$B$9)*$B$14</f>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" ref="K23:K52" si="3">IF(O23=2,MIN(E22,MAX(0,$B$19-SUM(H23:J23))),IF(O23=1,MIN(E22,MAX(0,0.8*$B$19-SUM(H23:J23))),0))</f>
-        <v>76710</v>
+        <v>0</v>
       </c>
       <c r="L23" s="3">
         <f t="shared" ref="L23:L62" si="4">SUM(H23:K23)</f>
-        <v>200000</v>
+        <v>29419.25</v>
       </c>
       <c r="M23" s="3">
         <f>MAX(0,L23-$B$19,0)</f>
@@ -1425,44 +1420,44 @@
       <c r="A24" s="1">
         <v>2</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="2" t="str">
         <f>IF(B23&lt;$B$2-1,B23+1," ")</f>
-        <v>66</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="C24" s="2">
         <f>IF(C23&lt;=$B$3-2,C23+1," ")</f>
         <v>68</v>
       </c>
       <c r="D24">
-        <v>-0.241957990089258</v>
+        <v>0.150113466853733</v>
       </c>
       <c r="E24" s="3">
         <f t="shared" si="0"/>
-        <v>1558450.7384077639</v>
+        <v>0</v>
       </c>
       <c r="F24" s="3">
         <f t="shared" ref="F24:F62" si="5">IF(C24&gt;=$B$10,$B$11*(1+$B$16)^(A24-1),0)</f>
-        <v>25153.499999999996</v>
+        <v>28904.999999999996</v>
       </c>
       <c r="G24" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>35276.399999999994</v>
       </c>
       <c r="H24" s="3">
         <f t="shared" si="2"/>
-        <v>25153.499999999996</v>
+        <v>35276.399999999994</v>
       </c>
       <c r="J24" s="4">
         <f>J23</f>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="3"/>
-        <v>76096.5</v>
+        <v>0</v>
       </c>
       <c r="L24" s="3">
         <f t="shared" si="4"/>
-        <v>200000</v>
+        <v>30279.649999999994</v>
       </c>
       <c r="M24" s="3">
         <f t="shared" ref="M24:M62" si="6">MAX(0,L24-$B$19)</f>
@@ -1470,7 +1465,7 @@
       </c>
       <c r="O24" s="1">
         <f t="shared" ref="O24:O62" si="7">IF(AND(B24&lt;&gt;" ",C24&lt;&gt;" "),2,IF(OR(B24&lt;&gt;" ",C24&lt;&gt;" "),1,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P24" s="3"/>
       <c r="Q24" s="3"/>
@@ -1488,35 +1483,35 @@
         <v>69</v>
       </c>
       <c r="D25">
-        <v>0.166816654155825</v>
+        <v>8.7493202088067601E-2</v>
       </c>
       <c r="E25" s="3">
         <f t="shared" si="0"/>
-        <v>1783676.5160428823</v>
+        <v>0</v>
       </c>
       <c r="F25" s="3">
         <f t="shared" si="5"/>
-        <v>25782.337499999998</v>
+        <v>29627.624999999996</v>
       </c>
       <c r="G25" s="3">
         <f t="shared" si="1"/>
-        <v>31468.319999999996</v>
+        <v>36158.31</v>
       </c>
       <c r="H25" s="3">
         <f t="shared" si="2"/>
-        <v>31468.319999999996</v>
+        <v>36158.31</v>
       </c>
       <c r="J25" s="4">
         <f t="shared" ref="J25:J52" si="10">J24</f>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="3"/>
-        <v>29781.680000000008</v>
+        <v>0</v>
       </c>
       <c r="L25" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>31161.559999999998</v>
       </c>
       <c r="M25" s="3">
         <f t="shared" si="6"/>
@@ -1542,35 +1537,35 @@
         <v>70</v>
       </c>
       <c r="D26">
-        <v>-2.6191091274449602E-2</v>
+        <v>0.117731437086462</v>
       </c>
       <c r="E26" s="3">
         <f t="shared" si="0"/>
-        <v>1708724.5195652628</v>
+        <v>0</v>
       </c>
       <c r="F26" s="3">
         <f t="shared" si="5"/>
-        <v>26426.895937499998</v>
+        <v>30368.315624999996</v>
       </c>
       <c r="G26" s="3">
         <f t="shared" si="1"/>
-        <v>32255.027999999995</v>
+        <v>37062.267749999999</v>
       </c>
       <c r="H26" s="3">
         <f t="shared" si="2"/>
-        <v>32255.027999999995</v>
+        <v>37062.267749999999</v>
       </c>
       <c r="J26" s="4">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="3"/>
-        <v>28994.972000000009</v>
+        <v>0</v>
       </c>
       <c r="L26" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>32065.517749999999</v>
       </c>
       <c r="M26" s="3">
         <f t="shared" si="6"/>
@@ -1596,35 +1591,35 @@
         <v>71</v>
       </c>
       <c r="D27">
-        <v>7.7803761370602603E-2</v>
+        <v>0.232602192708803</v>
       </c>
       <c r="E27" s="3">
         <f t="shared" si="0"/>
-        <v>1811287.9392137185</v>
+        <v>0</v>
       </c>
       <c r="F27" s="3">
         <f t="shared" si="5"/>
-        <v>27087.568335937493</v>
+        <v>31127.523515624995</v>
       </c>
       <c r="G27" s="3">
         <f t="shared" si="1"/>
-        <v>33061.403699999995</v>
+        <v>37988.824443749989</v>
       </c>
       <c r="H27" s="3">
         <f t="shared" si="2"/>
-        <v>33061.403699999995</v>
+        <v>37988.824443749989</v>
       </c>
       <c r="J27" s="4">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="3"/>
-        <v>28188.596300000005</v>
+        <v>0</v>
       </c>
       <c r="L27" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>32992.074443749989</v>
       </c>
       <c r="M27" s="3">
         <f t="shared" si="6"/>
@@ -1650,35 +1645,35 @@
         <v>72</v>
       </c>
       <c r="D28">
-        <v>-5.8992600288500001E-2</v>
+        <v>0.24869376451595099</v>
       </c>
       <c r="E28" s="3">
         <f t="shared" si="0"/>
-        <v>1678687.4517406863</v>
+        <v>0</v>
       </c>
       <c r="F28" s="3">
         <f t="shared" si="5"/>
-        <v>27764.757544335927</v>
+        <v>31905.711603515614</v>
       </c>
       <c r="G28" s="3">
         <f t="shared" si="1"/>
-        <v>33887.93879249999</v>
+        <v>38938.545054843737</v>
       </c>
       <c r="H28" s="3">
         <f t="shared" si="2"/>
-        <v>33887.93879249999</v>
+        <v>38938.545054843737</v>
       </c>
       <c r="J28" s="4">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="3"/>
-        <v>27362.061207499995</v>
+        <v>0</v>
       </c>
       <c r="L28" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>33941.795054843737</v>
       </c>
       <c r="M28" s="3">
         <f t="shared" si="6"/>
@@ -1704,35 +1699,35 @@
         <v>73</v>
       </c>
       <c r="D29">
-        <v>0.145588243622707</v>
+        <v>1.16492846804894E-2</v>
       </c>
       <c r="E29" s="3">
         <f t="shared" si="0"/>
-        <v>1892709.4943975259</v>
+        <v>0</v>
       </c>
       <c r="F29" s="3">
         <f t="shared" si="5"/>
-        <v>28458.876482944324</v>
+        <v>32703.354393603502</v>
       </c>
       <c r="G29" s="3">
         <f t="shared" si="1"/>
-        <v>34735.137262312484</v>
+        <v>39912.008681214829</v>
       </c>
       <c r="H29" s="3">
         <f t="shared" si="2"/>
-        <v>34735.137262312484</v>
+        <v>39912.008681214829</v>
       </c>
       <c r="J29" s="4">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="3"/>
-        <v>26514.862737687508</v>
+        <v>0</v>
       </c>
       <c r="L29" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>34915.258681214829</v>
       </c>
       <c r="M29" s="3">
         <f t="shared" si="6"/>
@@ -1758,35 +1753,35 @@
         <v>74</v>
       </c>
       <c r="D30">
-        <v>-6.9156387986826107E-2</v>
+        <v>0.17017647493215499</v>
       </c>
       <c r="E30" s="3">
         <f t="shared" si="0"/>
-        <v>1737943.6761696644</v>
+        <v>0</v>
       </c>
       <c r="F30" s="3">
         <f t="shared" si="5"/>
-        <v>29170.348395017936</v>
+        <v>33520.938253443594</v>
       </c>
       <c r="G30" s="3">
         <f t="shared" si="1"/>
-        <v>35603.5156938703</v>
+        <v>40909.808898245203</v>
       </c>
       <c r="H30" s="3">
         <f>IF(AND(B30&lt;&gt;" ",C30&lt;&gt;" "),F30+G30,IF(AND(B30=" ",C30=" ")," ",MAX(F30,G30)))</f>
-        <v>35603.5156938703</v>
+        <v>40909.808898245203</v>
       </c>
       <c r="J30" s="4">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="3"/>
-        <v>25646.484306129685</v>
+        <v>0</v>
       </c>
       <c r="L30" s="3">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>35913.058898245203</v>
       </c>
       <c r="M30" s="3">
         <f>MAX(0,L30-160000)</f>
@@ -1800,7 +1795,7 @@
       <c r="Q30" s="3"/>
       <c r="S30" s="4">
         <f>SUM(H30:K30)</f>
-        <v>160000</v>
+        <v>35913.058898245203</v>
       </c>
     </row>
     <row r="31" spans="1:19" s="15" customFormat="1">
@@ -1816,35 +1811,35 @@
         <v>75</v>
       </c>
       <c r="D31">
-        <v>0.19623548635910801</v>
+        <v>-2.1274384753009802E-3</v>
       </c>
       <c r="E31" s="17">
         <f t="shared" si="0"/>
-        <v>2049375.4188230142</v>
+        <v>0</v>
       </c>
       <c r="F31" s="3">
         <f t="shared" si="5"/>
-        <v>29899.607104893381</v>
+        <v>34358.96170977968</v>
       </c>
       <c r="G31" s="3">
         <f t="shared" si="1"/>
-        <v>36493.603586217054</v>
+        <v>41932.55412070133</v>
       </c>
       <c r="H31" s="17">
         <f t="shared" ref="H31:H62" si="11">IF(AND(B31&lt;&gt;" ",C31&lt;&gt;" "),F31+G31,IF(AND(B31=" ",C31=" ")," ",MAX(F31,G31)))</f>
-        <v>36493.603586217054</v>
+        <v>41932.55412070133</v>
       </c>
       <c r="J31" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K31" s="26">
         <f t="shared" si="3"/>
-        <v>24756.396413782961</v>
+        <v>0</v>
       </c>
       <c r="L31" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>36935.80412070133</v>
       </c>
       <c r="M31" s="17">
         <f t="shared" si="6"/>
@@ -1870,35 +1865,35 @@
         <v>76</v>
       </c>
       <c r="D32">
-        <v>6.6849214800481893E-2</v>
+        <v>4.9567601360287102E-2</v>
       </c>
       <c r="E32" s="17">
         <f t="shared" si="0"/>
-        <v>2160936.5436356873</v>
+        <v>0</v>
       </c>
       <c r="F32" s="3">
         <f t="shared" si="5"/>
-        <v>30647.097282515711</v>
+        <v>35217.935752524165</v>
       </c>
       <c r="G32" s="3">
         <f t="shared" si="1"/>
-        <v>37405.943675872477</v>
+        <v>42980.86797371885</v>
       </c>
       <c r="H32" s="17">
         <f t="shared" si="11"/>
-        <v>37405.943675872477</v>
+        <v>42980.86797371885</v>
       </c>
       <c r="J32" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K32" s="26">
         <f t="shared" si="3"/>
-        <v>23844.056324127538</v>
+        <v>0</v>
       </c>
       <c r="L32" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>37984.11797371885</v>
       </c>
       <c r="M32" s="17">
         <f t="shared" si="6"/>
@@ -1924,35 +1919,35 @@
         <v>77</v>
       </c>
       <c r="D33">
-        <v>0.277740325003693</v>
+        <v>-6.4726219196217294E-2</v>
       </c>
       <c r="E33" s="17">
         <f t="shared" si="0"/>
-        <v>2731844.1263661599</v>
+        <v>0</v>
       </c>
       <c r="F33" s="3">
         <f t="shared" si="5"/>
-        <v>31413.274714578602</v>
+        <v>36098.384146337266</v>
       </c>
       <c r="G33" s="3">
         <f t="shared" si="1"/>
-        <v>38341.092267769287</v>
+        <v>44055.389673061829</v>
       </c>
       <c r="H33" s="17">
         <f t="shared" si="11"/>
-        <v>38341.092267769287</v>
+        <v>44055.389673061829</v>
       </c>
       <c r="J33" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K33" s="26">
         <f t="shared" si="3"/>
-        <v>22908.907732230728</v>
+        <v>0</v>
       </c>
       <c r="L33" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>39058.639673061829</v>
       </c>
       <c r="M33" s="17">
         <f t="shared" si="6"/>
@@ -1978,35 +1973,35 @@
         <v>78</v>
       </c>
       <c r="D34">
-        <v>-0.197102274024261</v>
+        <v>0.15369382405227899</v>
       </c>
       <c r="E34" s="17">
         <f t="shared" si="0"/>
-        <v>2175767.5262516038</v>
+        <v>0</v>
       </c>
       <c r="F34" s="3">
         <f t="shared" si="5"/>
-        <v>32198.606582443066</v>
+        <v>37000.8437499957</v>
       </c>
       <c r="G34" s="3">
         <f t="shared" si="1"/>
-        <v>39299.619574463519</v>
+        <v>45156.774414888372</v>
       </c>
       <c r="H34" s="17">
         <f t="shared" si="11"/>
-        <v>39299.619574463519</v>
+        <v>45156.774414888372</v>
       </c>
       <c r="J34" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K34" s="26">
         <f t="shared" si="3"/>
-        <v>21950.380425536481</v>
+        <v>0</v>
       </c>
       <c r="L34" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>40160.024414888372</v>
       </c>
       <c r="M34" s="17">
         <f t="shared" si="6"/>
@@ -2032,35 +2027,35 @@
         <v>79</v>
       </c>
       <c r="D35">
-        <v>0.116764265945421</v>
+        <v>5.42928237824407E-2</v>
       </c>
       <c r="E35" s="17">
         <f t="shared" si="0"/>
-        <v>2406403.2341092606</v>
+        <v>0</v>
       </c>
       <c r="F35" s="3">
         <f t="shared" si="5"/>
-        <v>33003.571747004142</v>
+        <v>37925.864843745592</v>
       </c>
       <c r="G35" s="3">
         <f t="shared" si="1"/>
-        <v>40282.110063825101</v>
+        <v>46285.693775260574</v>
       </c>
       <c r="H35" s="17">
         <f t="shared" si="11"/>
-        <v>40282.110063825101</v>
+        <v>46285.693775260574</v>
       </c>
       <c r="J35" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K35" s="26">
         <f t="shared" si="3"/>
-        <v>20967.889936174906</v>
+        <v>0</v>
       </c>
       <c r="L35" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>41288.943775260574</v>
       </c>
       <c r="M35" s="17">
         <f t="shared" si="6"/>
@@ -2081,40 +2076,40 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C36" s="16">
+      <c r="C36" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>80</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D36">
-        <v>0.106403064185942</v>
+        <v>0.184096300329912</v>
       </c>
       <c r="E36" s="17">
         <f t="shared" si="0"/>
-        <v>2640367.1804607115</v>
+        <v>0</v>
       </c>
       <c r="F36" s="3">
         <f t="shared" si="5"/>
-        <v>33828.661040679246</v>
+        <v>38874.011464839226</v>
       </c>
       <c r="G36" s="3">
         <f t="shared" si="1"/>
-        <v>41289.162815420728</v>
-      </c>
-      <c r="H36" s="17">
+        <v>47442.836119642088</v>
+      </c>
+      <c r="H36" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>41289.162815420728</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J36" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K36" s="26">
         <f t="shared" si="3"/>
-        <v>19960.837184579286</v>
+        <v>0</v>
       </c>
       <c r="L36" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M36" s="17">
         <f t="shared" si="6"/>
@@ -2123,7 +2118,7 @@
       <c r="N36" s="17"/>
       <c r="O36" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P36" s="26"/>
     </row>
@@ -2135,40 +2130,40 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C37" s="16">
+      <c r="C37" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>81</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D37">
-        <v>-0.11473490397650001</v>
+        <v>3.09525733112746E-2</v>
       </c>
       <c r="E37" s="17">
         <f t="shared" si="0"/>
-        <v>2320668.069468047</v>
+        <v>0</v>
       </c>
       <c r="F37" s="3">
         <f t="shared" si="5"/>
-        <v>34674.377566696217</v>
+        <v>39845.861751460201</v>
       </c>
       <c r="G37" s="3">
         <f t="shared" si="1"/>
-        <v>42321.391885806246</v>
-      </c>
-      <c r="H37" s="17">
+        <v>48628.907022633131</v>
+      </c>
+      <c r="H37" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>42321.391885806246</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J37" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K37" s="26">
         <f t="shared" si="3"/>
-        <v>18928.608114193747</v>
+        <v>0</v>
       </c>
       <c r="L37" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M37" s="17">
         <f t="shared" si="6"/>
@@ -2177,7 +2172,7 @@
       <c r="N37" s="17"/>
       <c r="O37" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P37" s="26"/>
     </row>
@@ -2189,40 +2184,40 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C38" s="16">
+      <c r="C38" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>82</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D38">
-        <v>0.26058042113128599</v>
+        <v>8.7573446703673494E-2</v>
       </c>
       <c r="E38" s="17">
         <f t="shared" si="0"/>
-        <v>2902861.4374780962</v>
+        <v>0</v>
       </c>
       <c r="F38" s="3">
         <f t="shared" si="5"/>
-        <v>35541.23700586363</v>
+        <v>40842.008295246713</v>
       </c>
       <c r="G38" s="3">
         <f t="shared" si="1"/>
-        <v>43379.426682951409</v>
-      </c>
-      <c r="H38" s="17">
+        <v>49844.629698198973</v>
+      </c>
+      <c r="H38" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>43379.426682951409</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J38" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K38" s="26">
         <f t="shared" si="3"/>
-        <v>17870.573317048606</v>
+        <v>0</v>
       </c>
       <c r="L38" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M38" s="17">
         <f t="shared" si="6"/>
@@ -2231,7 +2226,7 @@
       <c r="N38" s="17"/>
       <c r="O38" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P38" s="26"/>
     </row>
@@ -2243,40 +2238,40 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C39" s="16">
+      <c r="C39" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>83</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D39">
-        <v>0.160379378686513</v>
+        <v>0.192347884931442</v>
       </c>
       <c r="E39" s="17">
         <f t="shared" si="0"/>
-        <v>3348942.3212760161</v>
+        <v>0</v>
       </c>
       <c r="F39" s="17">
         <f t="shared" si="5"/>
-        <v>36429.767931010218</v>
+        <v>41863.058502627879</v>
       </c>
       <c r="G39" s="17">
         <f t="shared" si="1"/>
-        <v>44463.912350025188</v>
-      </c>
-      <c r="H39" s="17">
+        <v>51090.74544065394</v>
+      </c>
+      <c r="H39" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>44463.912350025188</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J39" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K39" s="26">
         <f t="shared" si="3"/>
-        <v>16786.087649974797</v>
+        <v>0</v>
       </c>
       <c r="L39" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M39" s="17">
         <f t="shared" si="6"/>
@@ -2285,7 +2280,7 @@
       <c r="N39" s="17"/>
       <c r="O39" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P39" s="26"/>
     </row>
@@ -2297,40 +2292,40 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C40" s="16">
+      <c r="C40" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>84</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D40">
-        <v>0.17434531041547399</v>
+        <v>-8.6928308087205697E-2</v>
       </c>
       <c r="E40" s="17">
         <f t="shared" si="0"/>
-        <v>3914407.4462042046</v>
+        <v>0</v>
       </c>
       <c r="F40" s="17">
         <f t="shared" si="5"/>
-        <v>37340.512129285467</v>
+        <v>42909.634965193574</v>
       </c>
       <c r="G40" s="17">
         <f t="shared" si="1"/>
-        <v>45575.510158775811</v>
-      </c>
-      <c r="H40" s="17">
+        <v>52368.014076670283</v>
+      </c>
+      <c r="H40" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>45575.510158775811</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J40" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K40" s="26">
         <f t="shared" si="3"/>
-        <v>15674.489841224189</v>
+        <v>0</v>
       </c>
       <c r="L40" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M40" s="17">
         <f t="shared" si="6"/>
@@ -2339,7 +2334,7 @@
       <c r="N40" s="17"/>
       <c r="O40" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P40" s="26"/>
     </row>
@@ -2351,44 +2346,44 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C41" s="16">
+      <c r="C41" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>85</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D41">
-        <v>5.0555076741792401E-3</v>
+        <v>9.5898910009989402E-2</v>
       </c>
       <c r="E41" s="17">
         <f t="shared" si="0"/>
-        <v>3922100.8174501378</v>
+        <v>0</v>
       </c>
       <c r="F41" s="17">
         <f t="shared" si="5"/>
-        <v>38274.024932517605</v>
+        <v>43982.375839323409</v>
       </c>
       <c r="G41" s="17">
         <f t="shared" si="1"/>
-        <v>46714.897912745211</v>
-      </c>
-      <c r="H41" s="17">
+        <v>53677.214428587038</v>
+      </c>
+      <c r="H41" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>46714.897912745211</v>
-      </c>
-      <c r="I41" s="15">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I41" s="15" t="str">
         <f>IF(C41=" "," ",$B$9*$B$15)</f>
-        <v>2500</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J41" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K41" s="26">
         <f t="shared" si="3"/>
-        <v>12035.102087254782</v>
+        <v>0</v>
       </c>
       <c r="L41" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M41" s="17">
         <f t="shared" si="6"/>
@@ -2397,7 +2392,7 @@
       <c r="N41" s="17"/>
       <c r="O41" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P41" s="26"/>
     </row>
@@ -2409,44 +2404,44 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C42" s="16">
+      <c r="C42" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>86</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D42">
-        <v>9.1510263480075099E-2</v>
+        <v>5.6963899034304398E-2</v>
       </c>
       <c r="E42" s="17">
         <f t="shared" si="0"/>
-        <v>4269151.6039633779</v>
+        <v>0</v>
       </c>
       <c r="F42" s="17">
         <f t="shared" si="5"/>
-        <v>39230.875555830549</v>
+        <v>45081.935235306497</v>
       </c>
       <c r="G42" s="17">
         <f t="shared" si="1"/>
-        <v>47882.770360563838</v>
-      </c>
-      <c r="H42" s="17">
+        <v>55019.144789301718</v>
+      </c>
+      <c r="H42" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>47882.770360563838</v>
-      </c>
-      <c r="I42" s="15">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I42" s="15" t="str">
         <f>IF(C42=" "," ",$B$9*$B$15)</f>
-        <v>2500</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="J42" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K42" s="26">
         <f t="shared" si="3"/>
-        <v>10867.229639436177</v>
+        <v>0</v>
       </c>
       <c r="L42" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M42" s="17">
         <f t="shared" si="6"/>
@@ -2455,7 +2450,7 @@
       <c r="N42" s="17"/>
       <c r="O42" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P42" s="26"/>
     </row>
@@ -2467,44 +2462,44 @@
         <f t="shared" si="8"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="C43" s="16">
+      <c r="C43" s="16" t="str">
         <f t="shared" si="9"/>
-        <v>87</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="D43">
-        <v>9.6678713648679707E-2</v>
+        <v>5.1382001376739199E-2</v>
       </c>
       <c r="E43" s="17">
         <f t="shared" si="0"/>
-        <v>4671282.6303589772</v>
+        <v>0</v>
       </c>
       <c r="F43" s="17">
         <f t="shared" si="5"/>
-        <v>40211.64744472631</v>
+        <v>46208.983616189158</v>
       </c>
       <c r="G43" s="17">
         <f t="shared" si="1"/>
-        <v>49079.839619577928</v>
-      </c>
-      <c r="H43" s="17">
+        <v>56394.623409034255</v>
+      </c>
+      <c r="H43" s="17" t="str">
         <f t="shared" si="11"/>
-        <v>49079.839619577928</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="I43" s="15">
         <f>IF(C43&lt;&gt;" ",$B$15*$B$9,0)</f>
-        <v>2500</v>
+        <v>0</v>
       </c>
       <c r="J43" s="18">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K43" s="26">
         <f t="shared" si="3"/>
-        <v>9670.1603804220795</v>
+        <v>0</v>
       </c>
       <c r="L43" s="17">
         <f t="shared" si="4"/>
-        <v>160000</v>
+        <v>-4996.75</v>
       </c>
       <c r="M43" s="17">
         <f t="shared" si="6"/>
@@ -2513,7 +2508,7 @@
       <c r="N43" s="17"/>
       <c r="O43" s="15">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P43" s="26"/>
     </row>
@@ -2529,20 +2524,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D44" s="19">
-        <v>0.20703387688553901</v>
+      <c r="D44">
+        <v>6.3245114902691302E-2</v>
       </c>
       <c r="E44" s="21">
         <f t="shared" si="0"/>
-        <v>5638396.3833502745</v>
+        <v>0</v>
       </c>
       <c r="F44" s="21">
         <f t="shared" si="5"/>
-        <v>41216.938630844459</v>
+        <v>47364.208206593881</v>
       </c>
       <c r="G44" s="21">
         <f t="shared" si="1"/>
-        <v>50306.83561006737</v>
+        <v>57804.4889942601</v>
       </c>
       <c r="H44" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2554,7 +2549,7 @@
       </c>
       <c r="J44" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K44" s="25">
         <f t="shared" si="3"/>
@@ -2562,7 +2557,7 @@
       </c>
       <c r="L44" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M44" s="21">
         <f t="shared" si="6"/>
@@ -2587,20 +2582,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D45" s="19">
-        <v>0.19485426667484301</v>
+      <c r="D45">
+        <v>7.3094610078574304E-2</v>
       </c>
       <c r="E45" s="21">
         <f t="shared" si="0"/>
-        <v>6737061.9758500792</v>
+        <v>0</v>
       </c>
       <c r="F45" s="21">
         <f t="shared" si="5"/>
-        <v>42247.362096615572</v>
+        <v>48548.313411758725</v>
       </c>
       <c r="G45" s="21">
         <f t="shared" si="1"/>
-        <v>51564.506500319054</v>
+        <v>59249.601219116601</v>
       </c>
       <c r="H45" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2612,7 +2607,7 @@
       </c>
       <c r="J45" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K45" s="25">
         <f t="shared" si="3"/>
@@ -2620,7 +2615,7 @@
       </c>
       <c r="L45" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M45" s="21">
         <f t="shared" si="6"/>
@@ -2645,20 +2640,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D46" s="19">
-        <v>0.15688656278624299</v>
+      <c r="D46">
+        <v>0.16505812281424601</v>
       </c>
       <c r="E46" s="21">
         <f t="shared" si="0"/>
-        <v>7794016.4725190932</v>
+        <v>0</v>
       </c>
       <c r="F46" s="21">
         <f t="shared" si="5"/>
-        <v>43303.546149030961</v>
+        <v>49762.021247052697</v>
       </c>
       <c r="G46" s="21">
         <f t="shared" si="1"/>
-        <v>52853.619162827032</v>
+        <v>60730.841249594523</v>
       </c>
       <c r="H46" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2670,7 +2665,7 @@
       </c>
       <c r="J46" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K46" s="25">
         <f t="shared" si="3"/>
@@ -2678,7 +2673,7 @@
       </c>
       <c r="L46" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M46" s="21">
         <f t="shared" si="6"/>
@@ -2703,20 +2698,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D47" s="19">
-        <v>6.0163293229541399E-2</v>
+      <c r="D47">
+        <v>0.16568629248469399</v>
       </c>
       <c r="E47" s="21">
         <f t="shared" si="0"/>
-        <v>8262930.1709911358</v>
+        <v>0</v>
       </c>
       <c r="F47" s="21">
         <f t="shared" si="5"/>
-        <v>44386.134802756729</v>
+        <v>51006.071778229008</v>
       </c>
       <c r="G47" s="21">
         <f t="shared" si="1"/>
-        <v>54174.959641897702</v>
+        <v>62249.112280834379</v>
       </c>
       <c r="H47" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2728,7 +2723,7 @@
       </c>
       <c r="J47" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K47" s="25">
         <f t="shared" si="3"/>
@@ -2736,7 +2731,7 @@
       </c>
       <c r="L47" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M47" s="21">
         <f t="shared" si="6"/>
@@ -2761,20 +2756,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D48" s="19">
-        <v>0.110007644695564</v>
+      <c r="D48">
+        <v>-7.4094727980627106E-2</v>
       </c>
       <c r="E48" s="21">
         <f t="shared" si="0"/>
-        <v>9171915.6573857851</v>
+        <v>0</v>
       </c>
       <c r="F48" s="21">
         <f t="shared" si="5"/>
-        <v>45495.78817282564</v>
+        <v>52281.223572684721</v>
       </c>
       <c r="G48" s="21">
         <f t="shared" si="1"/>
-        <v>55529.333632945134</v>
+        <v>63805.340087855227</v>
       </c>
       <c r="H48" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2786,7 +2781,7 @@
       </c>
       <c r="J48" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K48" s="25">
         <f t="shared" si="3"/>
@@ -2794,7 +2789,7 @@
       </c>
       <c r="L48" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M48" s="21">
         <f t="shared" si="6"/>
@@ -2819,20 +2814,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D49" s="19">
-        <v>0.36309615822057001</v>
+      <c r="D49">
+        <v>-1.6473508414535699E-2</v>
       </c>
       <c r="E49" s="21">
         <f t="shared" si="0"/>
-        <v>12502202.996105658</v>
+        <v>0</v>
       </c>
       <c r="F49" s="21">
         <f t="shared" si="5"/>
-        <v>46633.182877146282</v>
+        <v>53588.254162001838</v>
       </c>
       <c r="G49" s="21">
         <f t="shared" si="1"/>
-        <v>56917.566973768764</v>
+        <v>65400.47359005161</v>
       </c>
       <c r="H49" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2844,7 +2839,7 @@
       </c>
       <c r="J49" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K49" s="25">
         <f t="shared" si="3"/>
@@ -2852,7 +2847,7 @@
       </c>
       <c r="L49" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M49" s="21">
         <f t="shared" si="6"/>
@@ -2877,20 +2872,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D50" s="19">
-        <v>0.112860953824353</v>
+      <c r="D50">
+        <v>0.16602394221427699</v>
       </c>
       <c r="E50" s="21">
         <f t="shared" si="0"/>
-        <v>13913213.551151827</v>
+        <v>0</v>
       </c>
       <c r="F50" s="21">
         <f t="shared" si="5"/>
-        <v>47799.012449074937</v>
+        <v>54927.960516051884</v>
       </c>
       <c r="G50" s="21">
         <f t="shared" si="1"/>
-        <v>58340.506148112981</v>
+        <v>67035.485429802895</v>
       </c>
       <c r="H50" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2902,7 +2897,7 @@
       </c>
       <c r="J50" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K50" s="25">
         <f t="shared" si="3"/>
@@ -2910,7 +2905,7 @@
       </c>
       <c r="L50" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M50" s="21">
         <f t="shared" si="6"/>
@@ -2935,20 +2930,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D51" s="19">
-        <v>0.34065121843441099</v>
+      <c r="D51">
+        <v>0.171044078296754</v>
       </c>
       <c r="E51" s="21">
         <f t="shared" si="0"/>
-        <v>18652766.699689854</v>
+        <v>0</v>
       </c>
       <c r="F51" s="21">
         <f t="shared" si="5"/>
-        <v>48993.987760301803</v>
+        <v>56301.159528953176</v>
       </c>
       <c r="G51" s="21">
         <f t="shared" si="1"/>
-        <v>59799.018801815801</v>
+        <v>68711.372565547965</v>
       </c>
       <c r="H51" s="21" t="str">
         <f t="shared" si="11"/>
@@ -2960,7 +2955,7 @@
       </c>
       <c r="J51" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K51" s="25">
         <f t="shared" si="3"/>
@@ -2968,7 +2963,7 @@
       </c>
       <c r="L51" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M51" s="21">
         <f t="shared" si="6"/>
@@ -2993,20 +2988,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D52" s="19">
-        <v>-2.3976349050905798E-3</v>
+      <c r="D52">
+        <v>-6.5140689547558001E-2</v>
       </c>
       <c r="E52" s="21">
         <f t="shared" si="0"/>
-        <v>18608044.175174166</v>
+        <v>0</v>
       </c>
       <c r="F52" s="21">
         <f t="shared" si="5"/>
-        <v>50218.83745430936</v>
+        <v>57708.688517177012</v>
       </c>
       <c r="G52" s="21">
         <f t="shared" si="1"/>
-        <v>61293.9942718612</v>
+        <v>70429.156879686663</v>
       </c>
       <c r="H52" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3018,7 +3013,7 @@
       </c>
       <c r="J52" s="24">
         <f t="shared" si="10"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="K52" s="25">
         <f t="shared" si="3"/>
@@ -3026,7 +3021,7 @@
       </c>
       <c r="L52" s="21">
         <f t="shared" si="4"/>
-        <v>98750</v>
+        <v>-4996.75</v>
       </c>
       <c r="M52" s="21">
         <f t="shared" si="6"/>
@@ -3051,20 +3046,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D53" s="19">
-        <v>0.44305567311162902</v>
+      <c r="D53">
+        <v>0.14982507437147499</v>
       </c>
       <c r="E53" s="21">
         <f t="shared" si="0"/>
-        <v>26852443.712496884</v>
+        <v>0</v>
       </c>
       <c r="F53" s="21">
         <f t="shared" si="5"/>
-        <v>51474.30839066708</v>
+        <v>59151.405730106424</v>
       </c>
       <c r="G53" s="21">
         <f t="shared" si="1"/>
-        <v>62826.344128657714</v>
+        <v>72189.885801678814</v>
       </c>
       <c r="H53" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3102,20 +3097,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D54" s="19">
-        <v>-0.20083714751930401</v>
+      <c r="D54">
+        <v>4.1042648442483502E-2</v>
       </c>
       <c r="E54" s="21">
         <f t="shared" si="0"/>
-        <v>21459475.513356339</v>
+        <v>0</v>
       </c>
       <c r="F54" s="21">
         <f t="shared" si="5"/>
-        <v>52761.166100433773</v>
+        <v>60630.190873359097</v>
       </c>
       <c r="G54" s="21">
         <f t="shared" si="1"/>
-        <v>64397.002731874178</v>
+        <v>73994.632946720812</v>
       </c>
       <c r="H54" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3153,20 +3148,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D55" s="19">
-        <v>2.38111740139124E-2</v>
+      <c r="D55">
+        <v>-2.72048942750685E-2</v>
       </c>
       <c r="E55" s="21">
         <f t="shared" si="0"/>
-        <v>21970450.81905216</v>
+        <v>0</v>
       </c>
       <c r="F55" s="21">
         <f t="shared" si="5"/>
-        <v>54080.195252944599</v>
+        <v>62145.945645193067</v>
       </c>
       <c r="G55" s="21">
         <f t="shared" si="1"/>
-        <v>66006.927800171019</v>
+        <v>75844.498770388818</v>
       </c>
       <c r="H55" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3204,20 +3199,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D56" s="19">
-        <v>-4.1418846603599201E-2</v>
+      <c r="D56">
+        <v>8.6942192062119707E-3</v>
       </c>
       <c r="E56" s="21">
         <f t="shared" si="0"/>
-        <v>21060460.086765919</v>
+        <v>0</v>
       </c>
       <c r="F56" s="21">
         <f t="shared" si="5"/>
-        <v>55432.200134268212</v>
+        <v>63699.594286322885</v>
       </c>
       <c r="G56" s="21">
         <f t="shared" si="1"/>
-        <v>67657.100995175293</v>
+        <v>77740.611239648526</v>
       </c>
       <c r="H56" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3255,20 +3250,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D57" s="19">
-        <v>-8.8343919233458995E-2</v>
+      <c r="D57">
+        <v>7.74182276305211E-3</v>
       </c>
       <c r="E57" s="21">
         <f t="shared" si="0"/>
-        <v>19199896.501841184</v>
+        <v>0</v>
       </c>
       <c r="F57" s="21">
         <f t="shared" si="5"/>
-        <v>56818.005137624918</v>
+        <v>65292.084143480955</v>
       </c>
       <c r="G57" s="21">
         <f t="shared" si="1"/>
-        <v>69348.528520054664</v>
+        <v>79684.126520639737</v>
       </c>
       <c r="H57" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3306,20 +3301,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D58" s="19">
-        <v>0.268442762697293</v>
+      <c r="D58">
+        <v>9.1933588414557593E-2</v>
       </c>
       <c r="E58" s="21">
         <f t="shared" si="0"/>
-        <v>24353969.762297522</v>
+        <v>0</v>
       </c>
       <c r="F58" s="21">
         <f t="shared" si="5"/>
-        <v>58238.455266065532</v>
+        <v>66924.386247067974</v>
       </c>
       <c r="G58" s="21">
         <f t="shared" si="1"/>
-        <v>71082.241733056027</v>
+        <v>81676.229683655722</v>
       </c>
       <c r="H58" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3357,20 +3352,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D59" s="19">
-        <v>2.4746358183762501E-2</v>
+      <c r="D59">
+        <v>0.19971972416191899</v>
       </c>
       <c r="E59" s="21">
         <f t="shared" si="0"/>
-        <v>24956641.821231861</v>
+        <v>0</v>
       </c>
       <c r="F59" s="21">
         <f t="shared" si="5"/>
-        <v>59694.416647717175</v>
+        <v>68597.495903244679</v>
       </c>
       <c r="G59" s="21">
         <f t="shared" si="1"/>
-        <v>72859.297776382431</v>
+        <v>83718.135425747125</v>
       </c>
       <c r="H59" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3408,20 +3403,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D60" s="19">
-        <v>0.17396076611516301</v>
+      <c r="D60">
+        <v>5.7524323304662499E-2</v>
       </c>
       <c r="E60" s="21">
         <f t="shared" si="0"/>
-        <v>29298118.352115072</v>
+        <v>0</v>
       </c>
       <c r="F60" s="21">
         <f t="shared" si="5"/>
-        <v>61186.7770639101</v>
+        <v>70312.433300825782</v>
       </c>
       <c r="G60" s="21">
         <f t="shared" si="1"/>
-        <v>74680.780220791989</v>
+        <v>85811.088811390786</v>
       </c>
       <c r="H60" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3459,20 +3454,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D61" s="19">
-        <v>-0.10790475953216699</v>
+      <c r="D61">
+        <v>2.1414772868603899E-2</v>
       </c>
       <c r="E61" s="21">
         <f t="shared" si="0"/>
-        <v>26136711.936585128</v>
+        <v>0</v>
       </c>
       <c r="F61" s="21">
         <f t="shared" si="5"/>
-        <v>62716.446490507835</v>
+        <v>72070.244133346408</v>
       </c>
       <c r="G61" s="21">
         <f t="shared" si="1"/>
-        <v>76547.799726311772</v>
+        <v>87956.366031675541</v>
       </c>
       <c r="H61" s="21" t="str">
         <f t="shared" si="11"/>
@@ -3510,20 +3505,20 @@
         <f t="shared" si="9"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="D62" s="19">
-        <v>1.35999610893674E-2</v>
+      <c r="D62">
+        <v>0.15059926476038901</v>
       </c>
       <c r="E62" s="21">
         <f t="shared" si="0"/>
-        <v>26492170.20192669</v>
+        <v>0</v>
       </c>
       <c r="F62" s="21">
         <f t="shared" si="5"/>
-        <v>64284.357652770537</v>
+        <v>73872.000236680076</v>
       </c>
       <c r="G62" s="21">
         <f t="shared" si="1"/>
-        <v>78461.494719469571</v>
+        <v>90155.275182467434</v>
       </c>
       <c r="H62" s="21" t="str">
         <f t="shared" si="11"/>

</xml_diff>

<commit_message>
Improved comments in Variable-spending model.
</commit_message>
<xml_diff>
--- a/Check Set-spending Cotton Retirement Plan R Model.xlsx
+++ b/Check Set-spending Cotton Retirement Plan R Model.xlsx
@@ -219,7 +219,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="302">
+  <cellStyleXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,8 +522,14 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -557,7 +563,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -576,8 +581,13 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="302">
+  <cellStyles count="308">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -729,6 +739,9 @@
     <cellStyle name="Followed Hyperlink" xfId="297" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="299" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="301" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="303" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="305" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="307" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -879,6 +892,9 @@
     <cellStyle name="Hyperlink" xfId="296" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="298" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="300" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="302" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="304" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="306" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1210,8 +1226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S106"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B18" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1360,13 +1376,13 @@
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="22">
+      <c r="B9" s="21">
         <v>100000</v>
       </c>
       <c r="D9"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
       <c r="F9"/>
-      <c r="G9" s="22"/>
+      <c r="G9" s="21"/>
       <c r="I9" s="3"/>
       <c r="L9" s="3"/>
       <c r="M9" s="1"/>
@@ -1557,7 +1573,7 @@
         <v>160000</v>
       </c>
       <c r="D21"/>
-      <c r="E21" s="22"/>
+      <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
       <c r="I21" s="3"/>
@@ -1569,23 +1585,18 @@
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="21">
         <v>4000000</v>
       </c>
       <c r="D22"/>
-      <c r="E22"/>
+      <c r="E22" s="21"/>
       <c r="F22"/>
-      <c r="G22" s="22"/>
+      <c r="G22" s="21"/>
       <c r="I22" s="3"/>
       <c r="L22" s="3"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
     </row>
-    <row r="25" spans="1:17">
-      <c r="B25" s="1">
-        <v>112000</v>
-      </c>
-    </row>
     <row r="26" spans="1:17">
       <c r="E26" s="8" t="s">
         <v>14</v>
@@ -1693,11 +1704,11 @@
         <v>2</v>
       </c>
       <c r="P28" s="3">
-        <f>IF(O28=2,$B$6*($B$22-$B$9)*$B$14,IF(O28=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" ref="P28:P67" si="4">IF(O28=2,$B$6*($B$22-$B$9)*$B$14,IF(O28=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
         <v>156000</v>
       </c>
       <c r="Q28" s="3">
-        <f>IF(O28=2,$B$21,IF(O28=1,0.8*$B$21,0))</f>
+        <f t="shared" ref="Q28:Q67" si="5">IF(O28=2,$B$21,IF(O28=1,0.8*$B$21,0))</f>
         <v>160000</v>
       </c>
     </row>
@@ -1721,7 +1732,7 @@
         <v>1033962.2867981958</v>
       </c>
       <c r="F29" s="3">
-        <f t="shared" ref="F29:F67" si="4">IF(C29&gt;=$B$10,$B$11*(1+$B$16)^(A29-1),0)</f>
+        <f t="shared" ref="F29:F67" si="6">IF(C29&gt;=$B$10,$B$11*(1+$B$16)^(A29-1),0)</f>
         <v>28904.999999999996</v>
       </c>
       <c r="G29" s="3">
@@ -1733,11 +1744,11 @@
         <v>28904.999999999996</v>
       </c>
       <c r="J29" s="4">
-        <f t="shared" ref="J29:J67" si="5">P29</f>
+        <f t="shared" ref="J29:J67" si="7">P29</f>
         <v>156000</v>
       </c>
       <c r="K29" s="5">
-        <f t="shared" ref="K29:K67" si="6">MAX(0,$Q29-SUM(H29:J29))</f>
+        <f t="shared" ref="K29:K67" si="8">MAX(0,$Q29-SUM(H29:J29))</f>
         <v>0</v>
       </c>
       <c r="L29" s="3">
@@ -1745,19 +1756,19 @@
         <v>184905</v>
       </c>
       <c r="M29" s="3">
-        <f t="shared" ref="M29:M67" si="7">MAX(0,L29-Q29,0)</f>
+        <f t="shared" ref="M29:M67" si="9">MAX(0,L29-Q29,0)</f>
         <v>24905</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" ref="O29:O67" si="8">IF(AND(B29&lt;&gt;" ",C29&lt;&gt;" "),2,IF(OR(B29&lt;&gt;" ",C29&lt;&gt;" "),1,0))</f>
+        <f t="shared" ref="O29:O67" si="10">IF(AND(B29&lt;&gt;" ",C29&lt;&gt;" "),2,IF(OR(B29&lt;&gt;" ",C29&lt;&gt;" "),1,0))</f>
         <v>2</v>
       </c>
       <c r="P29" s="3">
-        <f>IF(O29=2,$B$6*($B$22-$B$9)*$B$14,IF(O29=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q29" s="3">
-        <f>IF(O29=2,$B$21,IF(O29=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -1766,11 +1777,11 @@
         <v>3</v>
       </c>
       <c r="B30" s="2">
-        <f t="shared" ref="B30:B67" si="9">IF(B29&lt;$B$2-1,B29+1," ")</f>
+        <f t="shared" ref="B30:B67" si="11">IF(B29&lt;$B$2-1,B29+1," ")</f>
         <v>67</v>
       </c>
       <c r="C30" s="2">
-        <f t="shared" ref="C30:C67" si="10">IF(C29&lt;=$B$3-2,C29+1," ")</f>
+        <f t="shared" ref="C30:C67" si="12">IF(C29&lt;=$B$3-2,C29+1," ")</f>
         <v>69</v>
       </c>
       <c r="D30">
@@ -1781,7 +1792,7 @@
         <v>1152296.8260816333</v>
       </c>
       <c r="F30" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>29627.624999999996</v>
       </c>
       <c r="G30" s="3">
@@ -1793,11 +1804,11 @@
         <v>29627.624999999996</v>
       </c>
       <c r="J30" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K30" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L30" s="3">
@@ -1805,19 +1816,19 @@
         <v>185627.625</v>
       </c>
       <c r="M30" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>25627.625</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P30" s="3">
-        <f>IF(O30=2,$B$6*($B$22-$B$9)*$B$14,IF(O30=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q30" s="3">
-        <f>IF(O30=2,$B$21,IF(O30=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -1826,11 +1837,11 @@
         <v>4</v>
       </c>
       <c r="B31" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>68</v>
       </c>
       <c r="C31" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>70</v>
       </c>
       <c r="D31">
@@ -1841,7 +1852,7 @@
         <v>1358856.7444773642</v>
       </c>
       <c r="F31" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>30368.315624999996</v>
       </c>
       <c r="G31" s="3">
@@ -1853,11 +1864,11 @@
         <v>67430.583374999987</v>
       </c>
       <c r="J31" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K31" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L31" s="3">
@@ -1865,19 +1876,19 @@
         <v>223430.58337499999</v>
       </c>
       <c r="M31" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>63430.583374999987</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P31" s="3">
-        <f>IF(O31=2,$B$6*($B$22-$B$9)*$B$14,IF(O31=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q31" s="3">
-        <f>IF(O31=2,$B$21,IF(O31=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -1886,11 +1897,11 @@
         <v>5</v>
       </c>
       <c r="B32" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>69</v>
       </c>
       <c r="C32" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>71</v>
       </c>
       <c r="D32">
@@ -1901,7 +1912,7 @@
         <v>1755192.35609586</v>
       </c>
       <c r="F32" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>31127.523515624995</v>
       </c>
       <c r="G32" s="3">
@@ -1913,11 +1924,11 @@
         <v>69116.34795937498</v>
       </c>
       <c r="J32" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K32" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L32" s="3">
@@ -1925,19 +1936,19 @@
         <v>225116.34795937498</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>65116.34795937498</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P32" s="3">
-        <f>IF(O32=2,$B$6*($B$22-$B$9)*$B$14,IF(O32=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q32" s="3">
-        <f>IF(O32=2,$B$21,IF(O32=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -1946,11 +1957,11 @@
         <v>6</v>
       </c>
       <c r="B33" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>70</v>
       </c>
       <c r="C33" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>72</v>
       </c>
       <c r="D33">
@@ -1961,7 +1972,7 @@
         <v>2275165.7570659583</v>
       </c>
       <c r="F33" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>31905.711603515614</v>
       </c>
       <c r="G33" s="3">
@@ -1973,11 +1984,11 @@
         <v>70844.256658359343</v>
       </c>
       <c r="J33" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K33" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L33" s="3">
@@ -1985,19 +1996,19 @@
         <v>226844.25665835934</v>
       </c>
       <c r="M33" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>66844.256658359343</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P33" s="3">
-        <f>IF(O33=2,$B$6*($B$22-$B$9)*$B$14,IF(O33=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q33" s="3">
-        <f>IF(O33=2,$B$21,IF(O33=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2006,11 +2017,11 @@
         <v>7</v>
       </c>
       <c r="B34" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>71</v>
       </c>
       <c r="C34" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>73</v>
       </c>
       <c r="D34">
@@ -2021,7 +2032,7 @@
         <v>2371084.4936380526</v>
       </c>
       <c r="F34" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>32703.354393603502</v>
       </c>
       <c r="G34" s="3">
@@ -2033,11 +2044,11 @@
         <v>72615.363074818335</v>
       </c>
       <c r="J34" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K34" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L34" s="3">
@@ -2045,19 +2056,19 @@
         <v>228615.36307481834</v>
       </c>
       <c r="M34" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>68615.363074818335</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P34" s="3">
-        <f>IF(O34=2,$B$6*($B$22-$B$9)*$B$14,IF(O34=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q34" s="3">
-        <f>IF(O34=2,$B$21,IF(O34=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2066,11 +2077,11 @@
         <v>8</v>
       </c>
       <c r="B35" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>72</v>
       </c>
       <c r="C35" s="2">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>74</v>
       </c>
       <c r="D35">
@@ -2081,7 +2092,7 @@
         <v>2857003.6979604713</v>
       </c>
       <c r="F35" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>33520.938253443594</v>
       </c>
       <c r="G35" s="3">
@@ -2093,11 +2104,11 @@
         <v>74430.747151688789</v>
       </c>
       <c r="J35" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K35" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L35" s="3">
@@ -2105,36 +2116,33 @@
         <v>230430.74715168879</v>
       </c>
       <c r="M35" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>70430.747151688789</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P35" s="3">
-        <f>IF(O35=2,$B$6*($B$22-$B$9)*$B$14,IF(O35=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q35" s="3">
-        <f>IF(O35=2,$B$21,IF(O35=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
-      <c r="S35" s="4">
-        <f>SUM(H35:K35)</f>
-        <v>230430.74715168879</v>
-      </c>
+      <c r="S35" s="4"/>
     </row>
     <row r="36" spans="1:19" s="14" customFormat="1">
       <c r="A36" s="14">
         <v>9</v>
       </c>
       <c r="B36" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>73</v>
       </c>
       <c r="C36" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>75</v>
       </c>
       <c r="D36">
@@ -2145,7 +2153,7 @@
         <v>2923063.3184476183</v>
       </c>
       <c r="F36" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>34358.96170977968</v>
       </c>
       <c r="G36" s="3">
@@ -2153,15 +2161,15 @@
         <v>41932.55412070133</v>
       </c>
       <c r="H36" s="16">
-        <f t="shared" ref="H36:H67" si="11">IF(AND(B36&lt;&gt;" ",C36&lt;&gt;" "),F36+G36,IF(AND(B36=" ",C36=" ")," ",MAX(F36,G36)))</f>
+        <f t="shared" ref="H36:H67" si="13">IF(AND(B36&lt;&gt;" ",C36&lt;&gt;" "),F36+G36,IF(AND(B36=" ",C36=" ")," ",MAX(F36,G36)))</f>
         <v>76291.515830481017</v>
       </c>
       <c r="J36" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K36" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L36" s="16">
@@ -2169,20 +2177,20 @@
         <v>232291.51583048102</v>
       </c>
       <c r="M36" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>72291.515830481017</v>
       </c>
       <c r="N36" s="16"/>
       <c r="O36" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P36" s="3">
-        <f>IF(O36=2,$B$6*($B$22-$B$9)*$B$14,IF(O36=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q36" s="3">
-        <f>IF(O36=2,$B$21,IF(O36=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2191,11 +2199,11 @@
         <v>10</v>
       </c>
       <c r="B37" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>74</v>
       </c>
       <c r="C37" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>76</v>
       </c>
       <c r="D37">
@@ -2206,7 +2214,7 @@
         <v>3145829.2162180631</v>
       </c>
       <c r="F37" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>35217.935752524165</v>
       </c>
       <c r="G37" s="3">
@@ -2214,15 +2222,15 @@
         <v>42980.86797371885</v>
       </c>
       <c r="H37" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>78198.803726243015</v>
       </c>
       <c r="J37" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K37" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L37" s="16">
@@ -2230,20 +2238,20 @@
         <v>234198.80372624303</v>
       </c>
       <c r="M37" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>74198.80372624303</v>
       </c>
       <c r="N37" s="16"/>
       <c r="O37" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P37" s="3">
-        <f>IF(O37=2,$B$6*($B$22-$B$9)*$B$14,IF(O37=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q37" s="3">
-        <f>IF(O37=2,$B$21,IF(O37=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2252,11 +2260,11 @@
         <v>11</v>
       </c>
       <c r="B38" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>75</v>
       </c>
       <c r="C38" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>77</v>
       </c>
       <c r="D38">
@@ -2267,7 +2275,7 @@
         <v>3013436.2127778139</v>
       </c>
       <c r="F38" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>36098.384146337266</v>
       </c>
       <c r="G38" s="3">
@@ -2275,15 +2283,15 @@
         <v>44055.389673061829</v>
       </c>
       <c r="H38" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>80153.773819399095</v>
       </c>
       <c r="J38" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K38" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L38" s="16">
@@ -2291,20 +2299,20 @@
         <v>236153.7738193991</v>
       </c>
       <c r="M38" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>76153.773819399095</v>
       </c>
       <c r="N38" s="16"/>
       <c r="O38" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P38" s="3">
-        <f>IF(O38=2,$B$6*($B$22-$B$9)*$B$14,IF(O38=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q38" s="3">
-        <f>IF(O38=2,$B$21,IF(O38=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2313,11 +2321,11 @@
         <v>12</v>
       </c>
       <c r="B39" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>76</v>
       </c>
       <c r="C39" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>78</v>
       </c>
       <c r="D39">
@@ -2328,7 +2336,7 @@
         <v>3566752.7092367159</v>
       </c>
       <c r="F39" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37000.8437499957</v>
       </c>
       <c r="G39" s="3">
@@ -2336,15 +2344,15 @@
         <v>45156.774414888372</v>
       </c>
       <c r="H39" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>82157.618164884072</v>
       </c>
       <c r="J39" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K39" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L39" s="16">
@@ -2352,20 +2360,20 @@
         <v>238157.61816488407</v>
       </c>
       <c r="M39" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>78157.618164884072</v>
       </c>
       <c r="N39" s="16"/>
       <c r="O39" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P39" s="3">
-        <f>IF(O39=2,$B$6*($B$22-$B$9)*$B$14,IF(O39=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q39" s="3">
-        <f>IF(O39=2,$B$21,IF(O39=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2374,11 +2382,11 @@
         <v>13</v>
       </c>
       <c r="B40" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>77</v>
       </c>
       <c r="C40" s="15">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>79</v>
       </c>
       <c r="D40">
@@ -2389,7 +2397,7 @@
         <v>3844968.2561912704</v>
       </c>
       <c r="F40" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>37925.864843745592</v>
       </c>
       <c r="G40" s="3">
@@ -2397,15 +2405,15 @@
         <v>46285.693775260574</v>
       </c>
       <c r="H40" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>84211.558619006159</v>
       </c>
       <c r="J40" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>156000</v>
       </c>
       <c r="K40" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L40" s="16">
@@ -2413,20 +2421,20 @@
         <v>240211.55861900616</v>
       </c>
       <c r="M40" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>80211.558619006159</v>
       </c>
       <c r="N40" s="16"/>
       <c r="O40" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="P40" s="3">
-        <f>IF(O40=2,$B$6*($B$22-$B$9)*$B$14,IF(O40=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>156000</v>
       </c>
       <c r="Q40" s="3">
-        <f>IF(O40=2,$B$21,IF(O40=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>160000</v>
       </c>
     </row>
@@ -2435,11 +2443,11 @@
         <v>14</v>
       </c>
       <c r="B41" s="15">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>78</v>
       </c>
       <c r="C41" s="15" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v xml:space="preserve"> </v>
       </c>
       <c r="D41">
@@ -2450,7 +2458,7 @@
         <v>4595964.5144648347</v>
       </c>
       <c r="F41" s="3">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>38874.011464839226</v>
       </c>
       <c r="G41" s="3">
@@ -2458,15 +2466,15 @@
         <v>47442.836119642088</v>
       </c>
       <c r="H41" s="16">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>47442.836119642088</v>
       </c>
       <c r="J41" s="4">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>117000.00000000003</v>
       </c>
       <c r="K41" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="L41" s="16">
@@ -2474,2062 +2482,2062 @@
         <v>164442.83611964213</v>
       </c>
       <c r="M41" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>36442.836119642132</v>
       </c>
       <c r="N41" s="16"/>
       <c r="O41" s="14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="P41" s="3">
-        <f>IF(O41=2,$B$6*($B$22-$B$9)*$B$14,IF(O41=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+        <f t="shared" si="4"/>
         <v>117000.00000000003</v>
       </c>
       <c r="Q41" s="3">
-        <f>IF(O41=2,$B$21,IF(O41=1,0.8*$B$21,0))</f>
+        <f t="shared" si="5"/>
         <v>128000</v>
       </c>
     </row>
-    <row r="42" spans="1:19" s="23" customFormat="1">
-      <c r="A42" s="23">
+    <row r="42" spans="1:19" s="22" customFormat="1">
+      <c r="A42" s="22">
         <v>15</v>
       </c>
-      <c r="B42" s="24">
-        <f t="shared" si="9"/>
+      <c r="B42" s="23">
+        <f t="shared" si="11"/>
         <v>79</v>
       </c>
-      <c r="C42" s="24" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D42" s="25">
+      <c r="C42" s="23" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D42" s="24">
         <v>3.09525733112746E-2</v>
       </c>
-      <c r="E42" s="26">
+      <c r="E42" s="25">
         <f t="shared" si="0"/>
         <v>4777015.0615606988</v>
       </c>
-      <c r="F42" s="28">
-        <f t="shared" si="4"/>
+      <c r="F42" s="27">
+        <f t="shared" si="6"/>
         <v>39845.861751460201</v>
       </c>
-      <c r="G42" s="28">
+      <c r="G42" s="27">
         <f t="shared" si="1"/>
         <v>48628.907022633131</v>
       </c>
-      <c r="H42" s="26">
-        <f t="shared" si="11"/>
+      <c r="H42" s="25">
+        <f t="shared" si="13"/>
         <v>48628.907022633131</v>
       </c>
-      <c r="J42" s="29">
-        <f t="shared" si="5"/>
+      <c r="J42" s="28">
+        <f t="shared" si="7"/>
         <v>117000.00000000003</v>
       </c>
-      <c r="K42" s="27">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L42" s="26">
+      <c r="K42" s="26">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L42" s="25">
         <f t="shared" si="3"/>
         <v>165628.90702263315</v>
       </c>
-      <c r="M42" s="28">
-        <f t="shared" si="7"/>
+      <c r="M42" s="27">
+        <f t="shared" si="9"/>
         <v>37628.907022633153</v>
       </c>
-      <c r="N42" s="26"/>
-      <c r="O42" s="23">
-        <f t="shared" si="8"/>
+      <c r="N42" s="25"/>
+      <c r="O42" s="22">
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
-      <c r="P42" s="28">
-        <f>IF(O42=2,$B$6*($B$22-$B$9)*$B$14,IF(O42=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
+      <c r="P42" s="27">
+        <f t="shared" si="4"/>
         <v>117000.00000000003</v>
       </c>
-      <c r="Q42" s="28">
-        <f>IF(O42=2,$B$21,IF(O42=1,0.8*$B$21,0))</f>
+      <c r="Q42" s="27">
+        <f t="shared" si="5"/>
         <v>128000</v>
       </c>
     </row>
-    <row r="43" spans="1:19" s="14" customFormat="1">
-      <c r="A43" s="14">
+    <row r="43" spans="1:19" s="17" customFormat="1">
+      <c r="A43" s="17">
         <v>16</v>
       </c>
-      <c r="B43" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C43" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D43">
+      <c r="B43" s="18" t="str">
+        <f t="shared" si="11"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="C43" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D43" s="29">
         <v>8.7573446703673494E-2</v>
       </c>
-      <c r="E43" s="16">
+      <c r="E43" s="19">
         <f t="shared" si="0"/>
         <v>5195354.7354569305</v>
       </c>
-      <c r="F43" s="16">
-        <f t="shared" si="4"/>
+      <c r="F43" s="19">
+        <f t="shared" si="6"/>
         <v>40842.008295246713</v>
       </c>
-      <c r="G43" s="16">
+      <c r="G43" s="19">
         <f t="shared" si="1"/>
         <v>49844.629698198973</v>
       </c>
-      <c r="H43" s="16" t="str">
+      <c r="H43" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J43" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="19"/>
+      <c r="O43" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" s="17" customFormat="1">
+      <c r="A44" s="17">
+        <v>17</v>
+      </c>
+      <c r="B44" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J43" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L43" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M43" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N43" s="16"/>
-      <c r="O43" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P43" s="16">
-        <f>IF(O43=2,$B$6*($B$22-$B$9)*$B$14,IF(O43=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q43" s="3">
-        <f>IF(O43=2,$B$21,IF(O43=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" s="14" customFormat="1">
-      <c r="A44" s="14">
-        <v>17</v>
-      </c>
-      <c r="B44" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C44" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D44" s="29">
         <v>0.192347884931442</v>
       </c>
-      <c r="E44" s="16">
+      <c r="E44" s="19">
         <f t="shared" si="0"/>
         <v>6194670.2302906225</v>
       </c>
-      <c r="F44" s="16">
-        <f t="shared" si="4"/>
+      <c r="F44" s="19">
+        <f t="shared" si="6"/>
         <v>41863.058502627879</v>
       </c>
-      <c r="G44" s="16">
+      <c r="G44" s="19">
         <f t="shared" si="1"/>
         <v>51090.74544065394</v>
       </c>
-      <c r="H44" s="16" t="str">
+      <c r="H44" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J44" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L44" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M44" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N44" s="19"/>
+      <c r="O44" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" s="17" customFormat="1">
+      <c r="A45" s="17">
+        <v>18</v>
+      </c>
+      <c r="B45" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J44" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K44" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L44" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M44" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N44" s="16"/>
-      <c r="O44" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P44" s="16">
-        <f>IF(O44=2,$B$6*($B$22-$B$9)*$B$14,IF(O44=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q44" s="3">
-        <f>IF(O44=2,$B$21,IF(O44=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" s="14" customFormat="1">
-      <c r="A45" s="14">
-        <v>18</v>
-      </c>
-      <c r="B45" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C45" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D45" s="29">
         <v>-8.6928308087205697E-2</v>
       </c>
-      <c r="E45" s="16">
+      <c r="E45" s="19">
         <f t="shared" si="0"/>
         <v>5656178.0280132778</v>
       </c>
-      <c r="F45" s="16">
-        <f t="shared" si="4"/>
+      <c r="F45" s="19">
+        <f t="shared" si="6"/>
         <v>42909.634965193574</v>
       </c>
-      <c r="G45" s="16">
+      <c r="G45" s="19">
         <f t="shared" si="1"/>
         <v>52368.014076670283</v>
       </c>
-      <c r="H45" s="16" t="str">
+      <c r="H45" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="J45" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K45" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L45" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M45" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N45" s="19"/>
+      <c r="O45" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" s="17" customFormat="1">
+      <c r="A46" s="17">
+        <v>19</v>
+      </c>
+      <c r="B46" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="J45" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K45" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L45" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M45" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N45" s="16"/>
-      <c r="O45" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P45" s="16">
-        <f>IF(O45=2,$B$6*($B$22-$B$9)*$B$14,IF(O45=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q45" s="3">
-        <f>IF(O45=2,$B$21,IF(O45=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" s="14" customFormat="1">
-      <c r="A46" s="14">
-        <v>19</v>
-      </c>
-      <c r="B46" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C46" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D46" s="29">
         <v>9.5898910009989402E-2</v>
       </c>
-      <c r="E46" s="16">
+      <c r="E46" s="19">
         <f t="shared" si="0"/>
         <v>6198599.3357222024</v>
       </c>
-      <c r="F46" s="16">
-        <f t="shared" si="4"/>
+      <c r="F46" s="19">
+        <f t="shared" si="6"/>
         <v>43982.375839323409</v>
       </c>
-      <c r="G46" s="16">
+      <c r="G46" s="19">
         <f t="shared" si="1"/>
         <v>53677.214428587038</v>
       </c>
-      <c r="H46" s="16" t="str">
+      <c r="H46" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I46" s="17">
+        <f t="shared" ref="I46:I67" si="14">IF(C46&lt;&gt;" ",$B$15*$B$9,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J46" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K46" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L46" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M46" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N46" s="19"/>
+      <c r="O46" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" s="17" customFormat="1">
+      <c r="A47" s="17">
+        <v>20</v>
+      </c>
+      <c r="B47" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I46" s="14">
-        <f t="shared" ref="I46:I67" si="12">IF(C46&lt;&gt;" ",$B$15*$B$9,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J46" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K46" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L46" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M46" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N46" s="16"/>
-      <c r="O46" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P46" s="16">
-        <f>IF(O46=2,$B$6*($B$22-$B$9)*$B$14,IF(O46=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q46" s="3">
-        <f>IF(O46=2,$B$21,IF(O46=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" s="14" customFormat="1">
-      <c r="A47" s="14">
-        <v>20</v>
-      </c>
-      <c r="B47" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C47" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D47">
+      <c r="C47" s="18" t="str">
+        <f t="shared" si="12"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D47" s="29">
         <v>5.6963899034304398E-2</v>
       </c>
-      <c r="E47" s="16">
+      <c r="E47" s="19">
         <f t="shared" si="0"/>
         <v>6551695.722436389</v>
       </c>
-      <c r="F47" s="16">
-        <f t="shared" si="4"/>
+      <c r="F47" s="19">
+        <f t="shared" si="6"/>
         <v>45081.935235306497</v>
       </c>
-      <c r="G47" s="16">
+      <c r="G47" s="19">
         <f t="shared" si="1"/>
         <v>55019.144789301718</v>
       </c>
-      <c r="H47" s="16" t="str">
+      <c r="H47" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I47" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J47" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K47" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L47" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M47" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N47" s="19"/>
+      <c r="O47" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q47" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" s="17" customFormat="1">
+      <c r="A48" s="17">
+        <v>21</v>
+      </c>
+      <c r="B48" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I47" s="14">
+      <c r="C48" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J47" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K47" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L47" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M47" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N47" s="16"/>
-      <c r="O47" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P47" s="16">
-        <f>IF(O47=2,$B$6*($B$22-$B$9)*$B$14,IF(O47=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q47" s="3">
-        <f>IF(O47=2,$B$21,IF(O47=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" s="14" customFormat="1">
-      <c r="A48" s="14">
-        <v>21</v>
-      </c>
-      <c r="B48" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C48" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D48">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D48" s="29">
         <v>5.1382001376739199E-2</v>
       </c>
-      <c r="E48" s="16">
+      <c r="E48" s="19">
         <f t="shared" si="0"/>
         <v>6888334.9610665916</v>
       </c>
-      <c r="F48" s="16">
-        <f t="shared" si="4"/>
+      <c r="F48" s="19">
+        <f t="shared" si="6"/>
         <v>46208.983616189158</v>
       </c>
-      <c r="G48" s="16">
+      <c r="G48" s="19">
         <f t="shared" si="1"/>
         <v>56394.623409034255</v>
       </c>
-      <c r="H48" s="16" t="str">
+      <c r="H48" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I48" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J48" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K48" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L48" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M48" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N48" s="19"/>
+      <c r="O48" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q48" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" s="17" customFormat="1">
+      <c r="A49" s="17">
+        <v>22</v>
+      </c>
+      <c r="B49" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I48" s="14">
+      <c r="C49" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K48" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L48" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="16"/>
-      <c r="O48" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P48" s="16">
-        <f>IF(O48=2,$B$6*($B$22-$B$9)*$B$14,IF(O48=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q48" s="3">
-        <f>IF(O48=2,$B$21,IF(O48=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" s="14" customFormat="1">
-      <c r="A49" s="14">
-        <v>22</v>
-      </c>
-      <c r="B49" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C49" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D49">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D49" s="29">
         <v>6.3245114902691302E-2</v>
       </c>
-      <c r="E49" s="16">
+      <c r="E49" s="19">
         <f t="shared" si="0"/>
         <v>7323988.4971674746</v>
       </c>
-      <c r="F49" s="16">
-        <f t="shared" si="4"/>
+      <c r="F49" s="19">
+        <f t="shared" si="6"/>
         <v>47364.208206593881</v>
       </c>
-      <c r="G49" s="16">
+      <c r="G49" s="19">
         <f t="shared" si="1"/>
         <v>57804.4889942601</v>
       </c>
-      <c r="H49" s="16" t="str">
+      <c r="H49" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I49" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K49" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L49" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M49" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N49" s="19"/>
+      <c r="O49" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P49" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q49" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" s="17" customFormat="1">
+      <c r="A50" s="17">
+        <v>23</v>
+      </c>
+      <c r="B50" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I49" s="14">
+      <c r="C50" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J49" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K49" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L49" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M49" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N49" s="16"/>
-      <c r="O49" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P49" s="16">
-        <f>IF(O49=2,$B$6*($B$22-$B$9)*$B$14,IF(O49=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q49" s="3">
-        <f>IF(O49=2,$B$21,IF(O49=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" s="14" customFormat="1">
-      <c r="A50" s="14">
-        <v>23</v>
-      </c>
-      <c r="B50" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C50" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D50">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D50" s="29">
         <v>7.3094610078574304E-2</v>
       </c>
-      <c r="E50" s="16">
+      <c r="E50" s="19">
         <f t="shared" si="0"/>
         <v>7859332.5805878947</v>
       </c>
-      <c r="F50" s="16">
-        <f t="shared" si="4"/>
+      <c r="F50" s="19">
+        <f t="shared" si="6"/>
         <v>48548.313411758725</v>
       </c>
-      <c r="G50" s="16">
+      <c r="G50" s="19">
         <f t="shared" si="1"/>
         <v>59249.601219116601</v>
       </c>
-      <c r="H50" s="16" t="str">
+      <c r="H50" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I50" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K50" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L50" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M50" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N50" s="19"/>
+      <c r="O50" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P50" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q50" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" s="17" customFormat="1">
+      <c r="A51" s="17">
+        <v>24</v>
+      </c>
+      <c r="B51" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I50" s="14">
+      <c r="C51" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J50" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K50" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L50" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M50" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N50" s="16"/>
-      <c r="O50" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P50" s="16">
-        <f>IF(O50=2,$B$6*($B$22-$B$9)*$B$14,IF(O50=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q50" s="3">
-        <f>IF(O50=2,$B$21,IF(O50=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" s="14" customFormat="1">
-      <c r="A51" s="14">
-        <v>24</v>
-      </c>
-      <c r="B51" s="15" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C51" s="15" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D51">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D51" s="29">
         <v>0.16505812281424601</v>
       </c>
-      <c r="E51" s="16">
+      <c r="E51" s="19">
         <f t="shared" si="0"/>
         <v>9156579.262912577</v>
       </c>
-      <c r="F51" s="16">
-        <f t="shared" si="4"/>
+      <c r="F51" s="19">
+        <f t="shared" si="6"/>
         <v>49762.021247052697</v>
       </c>
-      <c r="G51" s="16">
+      <c r="G51" s="19">
         <f t="shared" si="1"/>
         <v>60730.841249594523</v>
       </c>
-      <c r="H51" s="16" t="str">
+      <c r="H51" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I51" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K51" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L51" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M51" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N51" s="19"/>
+      <c r="O51" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P51" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q51" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" s="17" customFormat="1">
+      <c r="A52" s="17">
+        <v>25</v>
+      </c>
+      <c r="B52" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I51" s="14">
+      <c r="C52" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J51" s="17">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K51" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L51" s="16">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M51" s="16">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N51" s="16"/>
-      <c r="O51" s="14">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P51" s="16">
-        <f>IF(O51=2,$B$6*($B$22-$B$9)*$B$14,IF(O51=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q51" s="3">
-        <f>IF(O51=2,$B$21,IF(O51=1,0.8*$B$21,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" s="18" customFormat="1">
-      <c r="A52" s="18">
-        <v>25</v>
-      </c>
-      <c r="B52" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C52" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D52">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D52" s="29">
         <v>0.16568629248469399</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="19">
         <f t="shared" si="0"/>
         <v>10673698.932826795</v>
       </c>
-      <c r="F52" s="20">
-        <f t="shared" si="4"/>
+      <c r="F52" s="19">
+        <f t="shared" si="6"/>
         <v>51006.071778229008</v>
       </c>
-      <c r="G52" s="20">
+      <c r="G52" s="19">
         <f t="shared" si="1"/>
         <v>62249.112280834379</v>
       </c>
-      <c r="H52" s="20" t="str">
+      <c r="H52" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I52" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K52" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L52" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M52" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N52" s="19"/>
+      <c r="O52" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P52" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q52" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" s="17" customFormat="1">
+      <c r="A53" s="17">
+        <v>26</v>
+      </c>
+      <c r="B53" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I52" s="18">
+      <c r="C53" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J52" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K52" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L52" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M52" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N52" s="20"/>
-      <c r="O52" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P52" s="20">
-        <f>IF(O52=2,$B$6*($B$22-$B$9)*$B$14,IF(O52=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q52" s="3">
-        <f>IF(O52=2,$B$25,IF(O52=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" s="18" customFormat="1">
-      <c r="A53" s="18">
-        <v>26</v>
-      </c>
-      <c r="B53" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C53" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D53">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D53" s="29">
         <v>-7.4094727980627106E-2</v>
       </c>
-      <c r="E53" s="20">
+      <c r="E53" s="19">
         <f t="shared" si="0"/>
         <v>9882834.1138518844</v>
       </c>
-      <c r="F53" s="20">
-        <f t="shared" si="4"/>
+      <c r="F53" s="19">
+        <f t="shared" si="6"/>
         <v>52281.223572684721</v>
       </c>
-      <c r="G53" s="20">
+      <c r="G53" s="19">
         <f t="shared" si="1"/>
         <v>63805.340087855227</v>
       </c>
-      <c r="H53" s="20" t="str">
+      <c r="H53" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I53" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K53" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L53" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M53" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N53" s="19"/>
+      <c r="O53" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P53" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q53" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" s="17" customFormat="1">
+      <c r="A54" s="17">
+        <v>27</v>
+      </c>
+      <c r="B54" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I53" s="18">
+      <c r="C54" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J53" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K53" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L53" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M53" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N53" s="20"/>
-      <c r="O53" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P53" s="20">
-        <f>IF(O53=2,$B$6*($B$22-$B$9)*$B$14,IF(O53=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q53" s="3">
-        <f>IF(O53=2,$B$25,IF(O53=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" s="18" customFormat="1">
-      <c r="A54" s="18">
-        <v>27</v>
-      </c>
-      <c r="B54" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C54" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D54">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D54" s="29">
         <v>-1.6473508414535699E-2</v>
       </c>
-      <c r="E54" s="20">
+      <c r="E54" s="19">
         <f t="shared" si="0"/>
         <v>9720029.1629178859</v>
       </c>
-      <c r="F54" s="20">
-        <f t="shared" si="4"/>
+      <c r="F54" s="19">
+        <f t="shared" si="6"/>
         <v>53588.254162001838</v>
       </c>
-      <c r="G54" s="20">
+      <c r="G54" s="19">
         <f t="shared" si="1"/>
         <v>65400.47359005161</v>
       </c>
-      <c r="H54" s="20" t="str">
+      <c r="H54" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I54" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L54" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M54" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N54" s="19"/>
+      <c r="O54" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P54" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q54" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="17" customFormat="1">
+      <c r="A55" s="17">
+        <v>28</v>
+      </c>
+      <c r="B55" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I54" s="18">
+      <c r="C55" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K54" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L54" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M54" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N54" s="20"/>
-      <c r="O54" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P54" s="20">
-        <f>IF(O54=2,$B$6*($B$22-$B$9)*$B$14,IF(O54=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q54" s="3">
-        <f>IF(O54=2,$B$25,IF(O54=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" s="18" customFormat="1">
-      <c r="A55" s="18">
-        <v>28</v>
-      </c>
-      <c r="B55" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C55" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D55">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D55" s="29">
         <v>0.16602394221427699</v>
       </c>
-      <c r="E55" s="20">
+      <c r="E55" s="19">
         <f t="shared" si="0"/>
         <v>11333786.722983252</v>
       </c>
-      <c r="F55" s="20">
-        <f t="shared" si="4"/>
+      <c r="F55" s="19">
+        <f t="shared" si="6"/>
         <v>54927.960516051884</v>
       </c>
-      <c r="G55" s="20">
+      <c r="G55" s="19">
         <f t="shared" si="1"/>
         <v>67035.485429802895</v>
       </c>
-      <c r="H55" s="20" t="str">
+      <c r="H55" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I55" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J55" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K55" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M55" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N55" s="19"/>
+      <c r="O55" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P55" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q55" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" s="17" customFormat="1">
+      <c r="A56" s="17">
+        <v>29</v>
+      </c>
+      <c r="B56" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I55" s="18">
+      <c r="C56" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J55" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K55" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L55" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M55" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N55" s="20"/>
-      <c r="O55" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P55" s="20">
-        <f>IF(O55=2,$B$6*($B$22-$B$9)*$B$14,IF(O55=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q55" s="3">
-        <f>IF(O55=2,$B$25,IF(O55=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" s="18" customFormat="1">
-      <c r="A56" s="18">
-        <v>29</v>
-      </c>
-      <c r="B56" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C56" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D56">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D56" s="29">
         <v>0.171044078296754</v>
       </c>
-      <c r="E56" s="20">
+      <c r="E56" s="19">
         <f t="shared" si="0"/>
         <v>13272363.82662791</v>
       </c>
-      <c r="F56" s="20">
-        <f t="shared" si="4"/>
+      <c r="F56" s="19">
+        <f t="shared" si="6"/>
         <v>56301.159528953176</v>
       </c>
-      <c r="G56" s="20">
+      <c r="G56" s="19">
         <f t="shared" si="1"/>
         <v>68711.372565547965</v>
       </c>
-      <c r="H56" s="20" t="str">
+      <c r="H56" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I56" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K56" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L56" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M56" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N56" s="19"/>
+      <c r="O56" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P56" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q56" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" s="17" customFormat="1">
+      <c r="A57" s="17">
+        <v>30</v>
+      </c>
+      <c r="B57" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I56" s="18">
+      <c r="C57" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J56" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K56" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L56" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M56" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N56" s="20"/>
-      <c r="O56" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P56" s="20">
-        <f>IF(O56=2,$B$6*($B$22-$B$9)*$B$14,IF(O56=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q56" s="3">
-        <f>IF(O56=2,$B$25,IF(O56=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" s="18" customFormat="1">
-      <c r="A57" s="18">
-        <v>30</v>
-      </c>
-      <c r="B57" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C57" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D57">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D57" s="29">
         <v>-6.5140689547558001E-2</v>
       </c>
-      <c r="E57" s="20">
+      <c r="E57" s="19">
         <f t="shared" si="0"/>
         <v>12407792.895035302</v>
       </c>
-      <c r="F57" s="20">
-        <f t="shared" si="4"/>
+      <c r="F57" s="19">
+        <f t="shared" si="6"/>
         <v>57708.688517177012</v>
       </c>
-      <c r="G57" s="20">
+      <c r="G57" s="19">
         <f t="shared" si="1"/>
         <v>70429.156879686663</v>
       </c>
-      <c r="H57" s="20" t="str">
+      <c r="H57" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I57" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K57" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L57" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M57" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N57" s="19"/>
+      <c r="O57" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P57" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q57" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" s="17" customFormat="1">
+      <c r="A58" s="17">
+        <v>31</v>
+      </c>
+      <c r="B58" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I57" s="18">
+      <c r="C58" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J57" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K57" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L57" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M57" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N57" s="20"/>
-      <c r="O57" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P57" s="20">
-        <f>IF(O57=2,$B$6*($B$22-$B$9)*$B$14,IF(O57=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q57" s="3">
-        <f>IF(O57=2,$B$25,IF(O57=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" s="18" customFormat="1">
-      <c r="A58" s="18">
-        <v>31</v>
-      </c>
-      <c r="B58" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C58" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D58">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D58" s="29">
         <v>0.14982507437147499</v>
       </c>
-      <c r="E58" s="20">
+      <c r="E58" s="19">
         <f t="shared" si="0"/>
         <v>14266791.388319826</v>
       </c>
-      <c r="F58" s="20">
-        <f t="shared" si="4"/>
+      <c r="F58" s="19">
+        <f t="shared" si="6"/>
         <v>59151.405730106424</v>
       </c>
-      <c r="G58" s="20">
+      <c r="G58" s="19">
         <f t="shared" si="1"/>
         <v>72189.885801678814</v>
       </c>
-      <c r="H58" s="20" t="str">
+      <c r="H58" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I58" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K58" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L58" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M58" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N58" s="19"/>
+      <c r="O58" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P58" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q58" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" s="17" customFormat="1">
+      <c r="A59" s="17">
+        <v>32</v>
+      </c>
+      <c r="B59" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I58" s="18">
+      <c r="C59" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J58" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K58" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L58" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M58" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N58" s="20"/>
-      <c r="O58" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P58" s="20">
-        <f>IF(O58=2,$B$6*($B$22-$B$9)*$B$14,IF(O58=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q58" s="3">
-        <f>IF(O58=2,$B$25,IF(O58=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" s="18" customFormat="1">
-      <c r="A59" s="18">
-        <v>32</v>
-      </c>
-      <c r="B59" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C59" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D59">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D59" s="29">
         <v>4.1042648442483502E-2</v>
       </c>
-      <c r="E59" s="20">
+      <c r="E59" s="19">
         <f t="shared" si="0"/>
         <v>14852338.291672887</v>
       </c>
-      <c r="F59" s="20">
-        <f t="shared" si="4"/>
+      <c r="F59" s="19">
+        <f t="shared" si="6"/>
         <v>60630.190873359097</v>
       </c>
-      <c r="G59" s="20">
+      <c r="G59" s="19">
         <f t="shared" si="1"/>
         <v>73994.632946720812</v>
       </c>
-      <c r="H59" s="20" t="str">
+      <c r="H59" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I59" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K59" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L59" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M59" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N59" s="19"/>
+      <c r="O59" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P59" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q59" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" s="17" customFormat="1">
+      <c r="A60" s="17">
+        <v>33</v>
+      </c>
+      <c r="B60" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I59" s="18">
+      <c r="C60" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J59" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K59" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L59" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M59" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N59" s="20"/>
-      <c r="O59" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P59" s="20">
-        <f>IF(O59=2,$B$6*($B$22-$B$9)*$B$14,IF(O59=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q59" s="3">
-        <f>IF(O59=2,$B$25,IF(O59=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" s="18" customFormat="1">
-      <c r="A60" s="18">
-        <v>33</v>
-      </c>
-      <c r="B60" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C60" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D60">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D60" s="29">
         <v>-2.72048942750685E-2</v>
       </c>
-      <c r="E60" s="20">
+      <c r="E60" s="19">
         <f t="shared" si="0"/>
         <v>14448281.998710375</v>
       </c>
-      <c r="F60" s="20">
-        <f t="shared" si="4"/>
+      <c r="F60" s="19">
+        <f t="shared" si="6"/>
         <v>62145.945645193067</v>
       </c>
-      <c r="G60" s="20">
+      <c r="G60" s="19">
         <f t="shared" si="1"/>
         <v>75844.498770388818</v>
       </c>
-      <c r="H60" s="20" t="str">
+      <c r="H60" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I60" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J60" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K60" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L60" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M60" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N60" s="19"/>
+      <c r="O60" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P60" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q60" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" s="17" customFormat="1">
+      <c r="A61" s="17">
+        <v>34</v>
+      </c>
+      <c r="B61" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I60" s="18">
+      <c r="C61" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J60" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K60" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L60" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M60" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N60" s="20"/>
-      <c r="O60" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P60" s="20">
-        <f>IF(O60=2,$B$6*($B$22-$B$9)*$B$14,IF(O60=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q60" s="3">
-        <f>IF(O60=2,$B$25,IF(O60=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" s="18" customFormat="1">
-      <c r="A61" s="18">
-        <v>34</v>
-      </c>
-      <c r="B61" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C61" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D61">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D61" s="29">
         <v>8.6942192062119707E-3</v>
       </c>
-      <c r="E61" s="20">
+      <c r="E61" s="19">
         <f t="shared" si="0"/>
         <v>14573898.529560331</v>
       </c>
-      <c r="F61" s="20">
-        <f t="shared" si="4"/>
+      <c r="F61" s="19">
+        <f t="shared" si="6"/>
         <v>63699.594286322885</v>
       </c>
-      <c r="G61" s="20">
+      <c r="G61" s="19">
         <f t="shared" si="1"/>
         <v>77740.611239648526</v>
       </c>
-      <c r="H61" s="20" t="str">
+      <c r="H61" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I61" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J61" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K61" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L61" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M61" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N61" s="19"/>
+      <c r="O61" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P61" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q61" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" s="17" customFormat="1">
+      <c r="A62" s="17">
+        <v>35</v>
+      </c>
+      <c r="B62" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I61" s="18">
+      <c r="C62" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J61" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K61" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L61" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M61" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N61" s="20"/>
-      <c r="O61" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P61" s="20">
-        <f>IF(O61=2,$B$6*($B$22-$B$9)*$B$14,IF(O61=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q61" s="3">
-        <f>IF(O61=2,$B$25,IF(O61=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" s="18" customFormat="1">
-      <c r="A62" s="18">
-        <v>35</v>
-      </c>
-      <c r="B62" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C62" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D62">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D62" s="29">
         <v>7.74182276305211E-3</v>
       </c>
-      <c r="E62" s="20">
+      <c r="E62" s="19">
         <f t="shared" si="0"/>
         <v>14686727.068942893</v>
       </c>
-      <c r="F62" s="20">
-        <f t="shared" si="4"/>
+      <c r="F62" s="19">
+        <f t="shared" si="6"/>
         <v>65292.084143480955</v>
       </c>
-      <c r="G62" s="20">
+      <c r="G62" s="19">
         <f t="shared" si="1"/>
         <v>79684.126520639737</v>
       </c>
-      <c r="H62" s="20" t="str">
+      <c r="H62" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I62" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J62" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K62" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L62" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M62" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N62" s="19"/>
+      <c r="O62" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P62" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q62" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" s="17" customFormat="1">
+      <c r="A63" s="17">
+        <v>36</v>
+      </c>
+      <c r="B63" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I62" s="18">
+      <c r="C63" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J62" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K62" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M62" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N62" s="20"/>
-      <c r="O62" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P62" s="20">
-        <f>IF(O62=2,$B$6*($B$22-$B$9)*$B$14,IF(O62=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q62" s="3">
-        <f>IF(O62=2,$B$25,IF(O62=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" s="18" customFormat="1">
-      <c r="A63" s="18">
-        <v>36</v>
-      </c>
-      <c r="B63" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C63" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D63">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D63" s="29">
         <v>9.1933588414557593E-2</v>
       </c>
-      <c r="E63" s="20">
+      <c r="E63" s="19">
         <f t="shared" si="0"/>
         <v>16036930.590456031</v>
       </c>
-      <c r="F63" s="20">
-        <f t="shared" si="4"/>
+      <c r="F63" s="19">
+        <f t="shared" si="6"/>
         <v>66924.386247067974</v>
       </c>
-      <c r="G63" s="20">
+      <c r="G63" s="19">
         <f t="shared" si="1"/>
         <v>81676.229683655722</v>
       </c>
-      <c r="H63" s="20" t="str">
+      <c r="H63" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I63" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K63" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L63" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M63" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N63" s="19"/>
+      <c r="O63" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P63" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q63" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" s="17" customFormat="1">
+      <c r="A64" s="17">
+        <v>37</v>
+      </c>
+      <c r="B64" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I63" s="18">
+      <c r="C64" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J63" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K63" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L63" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M63" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N63" s="20"/>
-      <c r="O63" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P63" s="20">
-        <f>IF(O63=2,$B$6*($B$22-$B$9)*$B$14,IF(O63=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q63" s="3">
-        <f>IF(O63=2,$B$25,IF(O63=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" s="18" customFormat="1">
-      <c r="A64" s="18">
-        <v>37</v>
-      </c>
-      <c r="B64" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C64" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D64">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D64" s="29">
         <v>0.19971972416191899</v>
       </c>
-      <c r="E64" s="20">
+      <c r="E64" s="19">
         <f t="shared" si="0"/>
         <v>19239821.944385752</v>
       </c>
-      <c r="F64" s="20">
-        <f t="shared" si="4"/>
+      <c r="F64" s="19">
+        <f t="shared" si="6"/>
         <v>68597.495903244679</v>
       </c>
-      <c r="G64" s="20">
+      <c r="G64" s="19">
         <f t="shared" si="1"/>
         <v>83718.135425747125</v>
       </c>
-      <c r="H64" s="20" t="str">
+      <c r="H64" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I64" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K64" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L64" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M64" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N64" s="19"/>
+      <c r="O64" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P64" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q64" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" s="17" customFormat="1">
+      <c r="A65" s="17">
+        <v>38</v>
+      </c>
+      <c r="B65" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I64" s="18">
+      <c r="C65" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J64" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K64" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L64" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M64" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N64" s="20"/>
-      <c r="O64" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P64" s="20">
-        <f>IF(O64=2,$B$6*($B$22-$B$9)*$B$14,IF(O64=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q64" s="3">
-        <f>IF(O64=2,$B$25,IF(O64=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" s="18" customFormat="1">
-      <c r="A65" s="18">
-        <v>38</v>
-      </c>
-      <c r="B65" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C65" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D65">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D65" s="29">
         <v>5.7524323304662499E-2</v>
       </c>
-      <c r="E65" s="20">
+      <c r="E65" s="19">
         <f t="shared" si="0"/>
         <v>20346579.682238739</v>
       </c>
-      <c r="F65" s="20">
-        <f t="shared" si="4"/>
+      <c r="F65" s="19">
+        <f t="shared" si="6"/>
         <v>70312.433300825782</v>
       </c>
-      <c r="G65" s="20">
+      <c r="G65" s="19">
         <f t="shared" si="1"/>
         <v>85811.088811390786</v>
       </c>
-      <c r="H65" s="20" t="str">
+      <c r="H65" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I65" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J65" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K65" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L65" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M65" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N65" s="19"/>
+      <c r="O65" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P65" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q65" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" s="17" customFormat="1">
+      <c r="A66" s="17">
+        <v>39</v>
+      </c>
+      <c r="B66" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I65" s="18">
+      <c r="C66" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J65" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K65" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L65" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M65" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N65" s="20"/>
-      <c r="O65" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P65" s="20">
-        <f>IF(O65=2,$B$6*($B$22-$B$9)*$B$14,IF(O65=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q65" s="3">
-        <f>IF(O65=2,$B$25,IF(O65=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" s="18" customFormat="1">
-      <c r="A66" s="18">
-        <v>39</v>
-      </c>
-      <c r="B66" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C66" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D66">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D66" s="29">
         <v>2.1414772868603899E-2</v>
       </c>
-      <c r="E66" s="20">
+      <c r="E66" s="19">
         <f t="shared" si="0"/>
         <v>20782297.064786833</v>
       </c>
-      <c r="F66" s="20">
-        <f t="shared" si="4"/>
+      <c r="F66" s="19">
+        <f t="shared" si="6"/>
         <v>72070.244133346408</v>
       </c>
-      <c r="G66" s="20">
+      <c r="G66" s="19">
         <f t="shared" si="1"/>
         <v>87956.366031675541</v>
       </c>
-      <c r="H66" s="20" t="str">
+      <c r="H66" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I66" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J66" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K66" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L66" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M66" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N66" s="19"/>
+      <c r="O66" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P66" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q66" s="19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" s="17" customFormat="1">
+      <c r="A67" s="17">
+        <v>40</v>
+      </c>
+      <c r="B67" s="18" t="str">
         <f t="shared" si="11"/>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I66" s="18">
+      <c r="C67" s="18" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J66" s="4">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="K66" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L66" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M66" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N66" s="20"/>
-      <c r="O66" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P66" s="20">
-        <f>IF(O66=2,$B$6*($B$22-$B$9)*$B$14,IF(O66=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q66" s="3">
-        <f>IF(O66=2,$B$25,IF(O66=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" s="18" customFormat="1">
-      <c r="A67" s="18">
-        <v>40</v>
-      </c>
-      <c r="B67" s="19" t="str">
-        <f t="shared" si="9"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="C67" s="19" t="str">
-        <f t="shared" si="10"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="D67">
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="D67" s="29">
         <v>0.15059926476038901</v>
       </c>
-      <c r="E67" s="20">
+      <c r="E67" s="19">
         <f t="shared" si="0"/>
         <v>23912095.722775724</v>
       </c>
-      <c r="F67" s="20">
-        <f t="shared" si="4"/>
+      <c r="F67" s="19">
+        <f t="shared" si="6"/>
         <v>73872.000236680076</v>
       </c>
-      <c r="G67" s="20">
+      <c r="G67" s="19">
         <f t="shared" si="1"/>
         <v>90155.275182467434</v>
       </c>
-      <c r="H67" s="20" t="str">
-        <f t="shared" si="11"/>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I67" s="18">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="J67" s="4">
+      <c r="H67" s="19" t="str">
+        <f t="shared" si="13"/>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="I67" s="17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="J67" s="30">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="K67" s="31">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="L67" s="19">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="M67" s="19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="N67" s="19"/>
+      <c r="O67" s="17">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="P67" s="19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q67" s="19">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K67" s="5">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="L67" s="20">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M67" s="3">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="N67" s="20"/>
-      <c r="O67" s="18">
-        <f t="shared" si="8"/>
-        <v>0</v>
-      </c>
-      <c r="P67" s="20">
-        <f>IF(O67=2,$B$6*($B$22-$B$9)*$B$14,IF(O67=1,0.75*$B$6*($B$22-$B$9)*$B$14,0))</f>
-        <v>0</v>
-      </c>
-      <c r="Q67" s="3">
-        <f>IF(O67=2,$B$25,IF(O67=1,0.8*$B$25,0))</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" s="18" customFormat="1">
-      <c r="B68" s="19"/>
-      <c r="C68" s="19"/>
-      <c r="D68" s="21"/>
-      <c r="E68" s="20"/>
-      <c r="F68" s="20"/>
-      <c r="K68" s="20"/>
-      <c r="M68" s="20"/>
-      <c r="N68" s="20"/>
-    </row>
-    <row r="69" spans="1:17" s="18" customFormat="1">
-      <c r="B69" s="19"/>
-      <c r="C69" s="19"/>
-      <c r="D69" s="21"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="K69" s="20"/>
-      <c r="M69" s="20"/>
-      <c r="N69" s="20"/>
-    </row>
-    <row r="70" spans="1:17" s="18" customFormat="1">
-      <c r="B70" s="19"/>
-      <c r="C70" s="19"/>
-      <c r="D70" s="21"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20"/>
-      <c r="K70" s="20"/>
-      <c r="M70" s="20"/>
-      <c r="N70" s="20"/>
-    </row>
-    <row r="71" spans="1:17" s="18" customFormat="1">
-      <c r="B71" s="19"/>
-      <c r="C71" s="19"/>
-      <c r="D71" s="21"/>
-      <c r="E71" s="20"/>
-      <c r="F71" s="20"/>
-      <c r="K71" s="20"/>
-      <c r="M71" s="20"/>
-      <c r="N71" s="20"/>
-    </row>
-    <row r="72" spans="1:17" s="18" customFormat="1">
-      <c r="B72" s="19"/>
-      <c r="C72" s="19"/>
-      <c r="D72" s="21"/>
-      <c r="E72" s="20"/>
-      <c r="F72" s="20"/>
-      <c r="K72" s="20"/>
-      <c r="M72" s="20"/>
-      <c r="N72" s="20"/>
-    </row>
-    <row r="73" spans="1:17" s="18" customFormat="1">
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-      <c r="D73" s="21"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-      <c r="K73" s="20"/>
-      <c r="M73" s="20"/>
-      <c r="N73" s="20"/>
-    </row>
-    <row r="74" spans="1:17" s="18" customFormat="1">
-      <c r="B74" s="19"/>
-      <c r="C74" s="19"/>
-      <c r="D74" s="21"/>
-      <c r="E74" s="20"/>
-      <c r="F74" s="20"/>
-      <c r="K74" s="20"/>
-      <c r="M74" s="20"/>
-      <c r="N74" s="20"/>
-    </row>
-    <row r="75" spans="1:17" s="18" customFormat="1">
-      <c r="B75" s="19"/>
-      <c r="C75" s="19"/>
-      <c r="D75" s="21"/>
-      <c r="E75" s="20"/>
-      <c r="F75" s="20"/>
-      <c r="K75" s="20"/>
-      <c r="M75" s="20"/>
-      <c r="N75" s="20"/>
-    </row>
-    <row r="76" spans="1:17" s="18" customFormat="1">
-      <c r="B76" s="19"/>
-      <c r="C76" s="19"/>
-      <c r="D76" s="21"/>
-      <c r="E76" s="20"/>
-      <c r="F76" s="20"/>
-      <c r="K76" s="20"/>
-      <c r="M76" s="20"/>
-      <c r="N76" s="20"/>
-    </row>
-    <row r="77" spans="1:17" s="18" customFormat="1">
-      <c r="B77" s="19"/>
-      <c r="C77" s="19"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="20"/>
-      <c r="F77" s="20"/>
-      <c r="K77" s="20"/>
-      <c r="M77" s="20"/>
-      <c r="N77" s="20"/>
-    </row>
-    <row r="78" spans="1:17" s="18" customFormat="1">
-      <c r="B78" s="19"/>
-      <c r="C78" s="19"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="20"/>
-      <c r="F78" s="20"/>
-      <c r="K78" s="20"/>
-      <c r="M78" s="20"/>
-      <c r="N78" s="20"/>
-    </row>
-    <row r="79" spans="1:17" s="18" customFormat="1">
-      <c r="B79" s="19"/>
-      <c r="C79" s="19"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="20"/>
-      <c r="F79" s="20"/>
-      <c r="K79" s="20"/>
-      <c r="M79" s="20"/>
-      <c r="N79" s="20"/>
-    </row>
-    <row r="80" spans="1:17" s="18" customFormat="1">
-      <c r="B80" s="19"/>
-      <c r="C80" s="19"/>
-      <c r="D80" s="21"/>
-      <c r="E80" s="20"/>
-      <c r="F80" s="20"/>
-      <c r="K80" s="20"/>
-      <c r="M80" s="20"/>
-      <c r="N80" s="20"/>
-    </row>
-    <row r="81" spans="2:14" s="18" customFormat="1">
-      <c r="B81" s="19"/>
-      <c r="C81" s="19"/>
-      <c r="D81" s="21"/>
-      <c r="E81" s="20"/>
-      <c r="F81" s="20"/>
-      <c r="K81" s="20"/>
-      <c r="M81" s="20"/>
-      <c r="N81" s="20"/>
-    </row>
-    <row r="82" spans="2:14" s="18" customFormat="1">
-      <c r="B82" s="19"/>
-      <c r="C82" s="19"/>
-      <c r="D82" s="21"/>
-      <c r="E82" s="20"/>
-      <c r="F82" s="20"/>
-      <c r="K82" s="20"/>
-      <c r="M82" s="20"/>
-      <c r="N82" s="20"/>
-    </row>
-    <row r="83" spans="2:14" s="18" customFormat="1">
-      <c r="B83" s="19"/>
-      <c r="C83" s="19"/>
-      <c r="D83" s="21"/>
-      <c r="E83" s="20"/>
-      <c r="F83" s="20"/>
-      <c r="K83" s="20"/>
-      <c r="M83" s="20"/>
-      <c r="N83" s="20"/>
-    </row>
-    <row r="84" spans="2:14" s="18" customFormat="1">
-      <c r="B84" s="19"/>
-      <c r="C84" s="19"/>
-      <c r="D84" s="21"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="K84" s="20"/>
-      <c r="M84" s="20"/>
-      <c r="N84" s="20"/>
-    </row>
-    <row r="85" spans="2:14" s="18" customFormat="1">
-      <c r="B85" s="19"/>
-      <c r="C85" s="19"/>
-      <c r="D85" s="21"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="K85" s="20"/>
-      <c r="M85" s="20"/>
-      <c r="N85" s="20"/>
-    </row>
-    <row r="86" spans="2:14" s="18" customFormat="1">
-      <c r="B86" s="19"/>
-      <c r="C86" s="19"/>
-      <c r="D86" s="21"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="K86" s="20"/>
-      <c r="M86" s="20"/>
-      <c r="N86" s="20"/>
-    </row>
-    <row r="87" spans="2:14" s="18" customFormat="1">
-      <c r="B87" s="19"/>
-      <c r="C87" s="19"/>
-      <c r="D87" s="21"/>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="K87" s="20"/>
-      <c r="M87" s="20"/>
-      <c r="N87" s="20"/>
-    </row>
-    <row r="88" spans="2:14" s="18" customFormat="1">
-      <c r="B88" s="19"/>
-      <c r="C88" s="19"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="K88" s="20"/>
-      <c r="M88" s="20"/>
-      <c r="N88" s="20"/>
-    </row>
-    <row r="89" spans="2:14" s="18" customFormat="1">
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="21"/>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="K89" s="20"/>
-      <c r="M89" s="20"/>
-      <c r="N89" s="20"/>
-    </row>
-    <row r="90" spans="2:14" s="18" customFormat="1">
-      <c r="B90" s="19"/>
-      <c r="C90" s="19"/>
-      <c r="D90" s="21"/>
-      <c r="E90" s="20"/>
-      <c r="F90" s="20"/>
-      <c r="K90" s="20"/>
-      <c r="M90" s="20"/>
-      <c r="N90" s="20"/>
-    </row>
-    <row r="91" spans="2:14" s="18" customFormat="1">
-      <c r="B91" s="19"/>
-      <c r="C91" s="19"/>
-      <c r="D91" s="21"/>
-      <c r="E91" s="20"/>
-      <c r="F91" s="20"/>
-      <c r="K91" s="20"/>
-      <c r="M91" s="20"/>
-      <c r="N91" s="20"/>
-    </row>
-    <row r="92" spans="2:14" s="18" customFormat="1">
-      <c r="B92" s="19"/>
-      <c r="C92" s="19"/>
-      <c r="D92" s="21"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="20"/>
-      <c r="K92" s="20"/>
-      <c r="M92" s="20"/>
-      <c r="N92" s="20"/>
-    </row>
-    <row r="93" spans="2:14" s="18" customFormat="1">
-      <c r="B93" s="19"/>
-      <c r="C93" s="19"/>
-      <c r="D93" s="21"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="20"/>
-      <c r="K93" s="20"/>
-      <c r="M93" s="20"/>
-      <c r="N93" s="20"/>
-    </row>
-    <row r="94" spans="2:14" s="18" customFormat="1">
-      <c r="B94" s="19"/>
-      <c r="C94" s="19"/>
-      <c r="D94" s="21"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="20"/>
-      <c r="K94" s="20"/>
-      <c r="M94" s="20"/>
-      <c r="N94" s="20"/>
-    </row>
-    <row r="95" spans="2:14" s="18" customFormat="1">
-      <c r="D95" s="21"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="20"/>
-      <c r="K95" s="20"/>
-      <c r="M95" s="20"/>
-      <c r="N95" s="20"/>
-    </row>
-    <row r="96" spans="2:14" s="18" customFormat="1">
-      <c r="D96" s="21"/>
-      <c r="E96" s="20"/>
-      <c r="F96" s="20"/>
-      <c r="K96" s="20"/>
-      <c r="M96" s="20"/>
-      <c r="N96" s="20"/>
-    </row>
-    <row r="97" spans="4:14" s="18" customFormat="1">
-      <c r="D97" s="21"/>
-      <c r="E97" s="20"/>
-      <c r="F97" s="20"/>
-      <c r="K97" s="20"/>
-      <c r="M97" s="20"/>
-      <c r="N97" s="20"/>
-    </row>
-    <row r="98" spans="4:14" s="18" customFormat="1">
-      <c r="D98" s="21"/>
-      <c r="E98" s="20"/>
-      <c r="F98" s="20"/>
-      <c r="K98" s="20"/>
-      <c r="M98" s="20"/>
-      <c r="N98" s="20"/>
-    </row>
-    <row r="99" spans="4:14" s="18" customFormat="1">
-      <c r="D99" s="21"/>
-      <c r="E99" s="20"/>
-      <c r="F99" s="20"/>
-      <c r="K99" s="20"/>
-      <c r="M99" s="20"/>
-      <c r="N99" s="20"/>
-    </row>
-    <row r="100" spans="4:14" s="18" customFormat="1">
-      <c r="D100" s="21"/>
-      <c r="E100" s="20"/>
-      <c r="F100" s="20"/>
-      <c r="K100" s="20"/>
-      <c r="M100" s="20"/>
-      <c r="N100" s="20"/>
-    </row>
-    <row r="101" spans="4:14" s="18" customFormat="1">
-      <c r="D101" s="21"/>
-      <c r="E101" s="20"/>
-      <c r="F101" s="20"/>
-      <c r="K101" s="20"/>
-      <c r="M101" s="20"/>
-      <c r="N101" s="20"/>
-    </row>
-    <row r="102" spans="4:14" s="18" customFormat="1">
-      <c r="D102" s="21"/>
-      <c r="E102" s="20"/>
-      <c r="F102" s="20"/>
-      <c r="K102" s="20"/>
-      <c r="M102" s="20"/>
-      <c r="N102" s="20"/>
-    </row>
-    <row r="103" spans="4:14" s="18" customFormat="1">
-      <c r="D103" s="21"/>
-      <c r="E103" s="20"/>
-      <c r="F103" s="20"/>
-      <c r="K103" s="20"/>
-      <c r="M103" s="20"/>
-      <c r="N103" s="20"/>
-    </row>
-    <row r="104" spans="4:14" s="18" customFormat="1">
-      <c r="D104" s="21"/>
-      <c r="E104" s="20"/>
-      <c r="F104" s="20"/>
-      <c r="K104" s="20"/>
-      <c r="M104" s="20"/>
-      <c r="N104" s="20"/>
-    </row>
-    <row r="105" spans="4:14" s="18" customFormat="1">
-      <c r="D105" s="21"/>
-      <c r="E105" s="20"/>
-      <c r="F105" s="20"/>
-      <c r="K105" s="20"/>
-      <c r="M105" s="20"/>
-      <c r="N105" s="20"/>
-    </row>
-    <row r="106" spans="4:14" s="18" customFormat="1">
-      <c r="D106" s="21"/>
-      <c r="E106" s="20"/>
-      <c r="F106" s="20"/>
-      <c r="K106" s="20"/>
-      <c r="M106" s="20"/>
-      <c r="N106" s="20"/>
+    </row>
+    <row r="68" spans="1:17" s="17" customFormat="1">
+      <c r="B68" s="18"/>
+      <c r="C68" s="18"/>
+      <c r="D68" s="20"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="19"/>
+      <c r="K68" s="19"/>
+      <c r="M68" s="19"/>
+      <c r="N68" s="19"/>
+    </row>
+    <row r="69" spans="1:17" s="17" customFormat="1">
+      <c r="B69" s="18"/>
+      <c r="C69" s="18"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="K69" s="19"/>
+      <c r="M69" s="19"/>
+      <c r="N69" s="19"/>
+    </row>
+    <row r="70" spans="1:17" s="17" customFormat="1">
+      <c r="B70" s="18"/>
+      <c r="C70" s="18"/>
+      <c r="D70" s="20"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19"/>
+      <c r="K70" s="19"/>
+      <c r="M70" s="19"/>
+      <c r="N70" s="19"/>
+    </row>
+    <row r="71" spans="1:17" s="17" customFormat="1">
+      <c r="B71" s="18"/>
+      <c r="C71" s="18"/>
+      <c r="D71" s="20"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="K71" s="19"/>
+      <c r="M71" s="19"/>
+      <c r="N71" s="19"/>
+    </row>
+    <row r="72" spans="1:17" s="17" customFormat="1">
+      <c r="B72" s="18"/>
+      <c r="C72" s="18"/>
+      <c r="D72" s="20"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19"/>
+      <c r="K72" s="19"/>
+      <c r="M72" s="19"/>
+      <c r="N72" s="19"/>
+    </row>
+    <row r="73" spans="1:17" s="17" customFormat="1">
+      <c r="B73" s="18"/>
+      <c r="C73" s="18"/>
+      <c r="D73" s="20"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19"/>
+      <c r="K73" s="19"/>
+      <c r="M73" s="19"/>
+      <c r="N73" s="19"/>
+    </row>
+    <row r="74" spans="1:17" s="17" customFormat="1">
+      <c r="B74" s="18"/>
+      <c r="C74" s="18"/>
+      <c r="D74" s="20"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19"/>
+      <c r="K74" s="19"/>
+      <c r="M74" s="19"/>
+      <c r="N74" s="19"/>
+    </row>
+    <row r="75" spans="1:17" s="17" customFormat="1">
+      <c r="B75" s="18"/>
+      <c r="C75" s="18"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+      <c r="K75" s="19"/>
+      <c r="M75" s="19"/>
+      <c r="N75" s="19"/>
+    </row>
+    <row r="76" spans="1:17" s="17" customFormat="1">
+      <c r="B76" s="18"/>
+      <c r="C76" s="18"/>
+      <c r="D76" s="20"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+      <c r="K76" s="19"/>
+      <c r="M76" s="19"/>
+      <c r="N76" s="19"/>
+    </row>
+    <row r="77" spans="1:17" s="17" customFormat="1">
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19"/>
+      <c r="K77" s="19"/>
+      <c r="M77" s="19"/>
+      <c r="N77" s="19"/>
+    </row>
+    <row r="78" spans="1:17" s="17" customFormat="1">
+      <c r="B78" s="18"/>
+      <c r="C78" s="18"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19"/>
+      <c r="K78" s="19"/>
+      <c r="M78" s="19"/>
+      <c r="N78" s="19"/>
+    </row>
+    <row r="79" spans="1:17" s="17" customFormat="1">
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+      <c r="D79" s="20"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19"/>
+      <c r="K79" s="19"/>
+      <c r="M79" s="19"/>
+      <c r="N79" s="19"/>
+    </row>
+    <row r="80" spans="1:17" s="17" customFormat="1">
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+      <c r="D80" s="20"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19"/>
+      <c r="K80" s="19"/>
+      <c r="M80" s="19"/>
+      <c r="N80" s="19"/>
+    </row>
+    <row r="81" spans="2:14" s="17" customFormat="1">
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19"/>
+      <c r="K81" s="19"/>
+      <c r="M81" s="19"/>
+      <c r="N81" s="19"/>
+    </row>
+    <row r="82" spans="2:14" s="17" customFormat="1">
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+      <c r="D82" s="20"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19"/>
+      <c r="K82" s="19"/>
+      <c r="M82" s="19"/>
+      <c r="N82" s="19"/>
+    </row>
+    <row r="83" spans="2:14" s="17" customFormat="1">
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+      <c r="D83" s="20"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="K83" s="19"/>
+      <c r="M83" s="19"/>
+      <c r="N83" s="19"/>
+    </row>
+    <row r="84" spans="2:14" s="17" customFormat="1">
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+      <c r="D84" s="20"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="K84" s="19"/>
+      <c r="M84" s="19"/>
+      <c r="N84" s="19"/>
+    </row>
+    <row r="85" spans="2:14" s="17" customFormat="1">
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+      <c r="D85" s="20"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="K85" s="19"/>
+      <c r="M85" s="19"/>
+      <c r="N85" s="19"/>
+    </row>
+    <row r="86" spans="2:14" s="17" customFormat="1">
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+      <c r="D86" s="20"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="K86" s="19"/>
+      <c r="M86" s="19"/>
+      <c r="N86" s="19"/>
+    </row>
+    <row r="87" spans="2:14" s="17" customFormat="1">
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+      <c r="D87" s="20"/>
+      <c r="E87" s="19"/>
+      <c r="F87" s="19"/>
+      <c r="K87" s="19"/>
+      <c r="M87" s="19"/>
+      <c r="N87" s="19"/>
+    </row>
+    <row r="88" spans="2:14" s="17" customFormat="1">
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
+      <c r="K88" s="19"/>
+      <c r="M88" s="19"/>
+      <c r="N88" s="19"/>
+    </row>
+    <row r="89" spans="2:14" s="17" customFormat="1">
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
+      <c r="K89" s="19"/>
+      <c r="M89" s="19"/>
+      <c r="N89" s="19"/>
+    </row>
+    <row r="90" spans="2:14" s="17" customFormat="1">
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
+      <c r="K90" s="19"/>
+      <c r="M90" s="19"/>
+      <c r="N90" s="19"/>
+    </row>
+    <row r="91" spans="2:14" s="17" customFormat="1">
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+      <c r="D91" s="20"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
+      <c r="K91" s="19"/>
+      <c r="M91" s="19"/>
+      <c r="N91" s="19"/>
+    </row>
+    <row r="92" spans="2:14" s="17" customFormat="1">
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+      <c r="D92" s="20"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
+      <c r="K92" s="19"/>
+      <c r="M92" s="19"/>
+      <c r="N92" s="19"/>
+    </row>
+    <row r="93" spans="2:14" s="17" customFormat="1">
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+      <c r="D93" s="20"/>
+      <c r="E93" s="19"/>
+      <c r="F93" s="19"/>
+      <c r="K93" s="19"/>
+      <c r="M93" s="19"/>
+      <c r="N93" s="19"/>
+    </row>
+    <row r="94" spans="2:14" s="17" customFormat="1">
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+      <c r="D94" s="20"/>
+      <c r="E94" s="19"/>
+      <c r="F94" s="19"/>
+      <c r="K94" s="19"/>
+      <c r="M94" s="19"/>
+      <c r="N94" s="19"/>
+    </row>
+    <row r="95" spans="2:14" s="17" customFormat="1">
+      <c r="D95" s="20"/>
+      <c r="E95" s="19"/>
+      <c r="F95" s="19"/>
+      <c r="K95" s="19"/>
+      <c r="M95" s="19"/>
+      <c r="N95" s="19"/>
+    </row>
+    <row r="96" spans="2:14" s="17" customFormat="1">
+      <c r="D96" s="20"/>
+      <c r="E96" s="19"/>
+      <c r="F96" s="19"/>
+      <c r="K96" s="19"/>
+      <c r="M96" s="19"/>
+      <c r="N96" s="19"/>
+    </row>
+    <row r="97" spans="4:14" s="17" customFormat="1">
+      <c r="D97" s="20"/>
+      <c r="E97" s="19"/>
+      <c r="F97" s="19"/>
+      <c r="K97" s="19"/>
+      <c r="M97" s="19"/>
+      <c r="N97" s="19"/>
+    </row>
+    <row r="98" spans="4:14" s="17" customFormat="1">
+      <c r="D98" s="20"/>
+      <c r="E98" s="19"/>
+      <c r="F98" s="19"/>
+      <c r="K98" s="19"/>
+      <c r="M98" s="19"/>
+      <c r="N98" s="19"/>
+    </row>
+    <row r="99" spans="4:14" s="17" customFormat="1">
+      <c r="D99" s="20"/>
+      <c r="E99" s="19"/>
+      <c r="F99" s="19"/>
+      <c r="K99" s="19"/>
+      <c r="M99" s="19"/>
+      <c r="N99" s="19"/>
+    </row>
+    <row r="100" spans="4:14" s="17" customFormat="1">
+      <c r="D100" s="20"/>
+      <c r="E100" s="19"/>
+      <c r="F100" s="19"/>
+      <c r="K100" s="19"/>
+      <c r="M100" s="19"/>
+      <c r="N100" s="19"/>
+    </row>
+    <row r="101" spans="4:14" s="17" customFormat="1">
+      <c r="D101" s="20"/>
+      <c r="E101" s="19"/>
+      <c r="F101" s="19"/>
+      <c r="K101" s="19"/>
+      <c r="M101" s="19"/>
+      <c r="N101" s="19"/>
+    </row>
+    <row r="102" spans="4:14" s="17" customFormat="1">
+      <c r="D102" s="20"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="19"/>
+      <c r="K102" s="19"/>
+      <c r="M102" s="19"/>
+      <c r="N102" s="19"/>
+    </row>
+    <row r="103" spans="4:14" s="17" customFormat="1">
+      <c r="D103" s="20"/>
+      <c r="E103" s="19"/>
+      <c r="F103" s="19"/>
+      <c r="K103" s="19"/>
+      <c r="M103" s="19"/>
+      <c r="N103" s="19"/>
+    </row>
+    <row r="104" spans="4:14" s="17" customFormat="1">
+      <c r="D104" s="20"/>
+      <c r="E104" s="19"/>
+      <c r="F104" s="19"/>
+      <c r="K104" s="19"/>
+      <c r="M104" s="19"/>
+      <c r="N104" s="19"/>
+    </row>
+    <row r="105" spans="4:14" s="17" customFormat="1">
+      <c r="D105" s="20"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19"/>
+      <c r="K105" s="19"/>
+      <c r="M105" s="19"/>
+      <c r="N105" s="19"/>
+    </row>
+    <row r="106" spans="4:14" s="17" customFormat="1">
+      <c r="D106" s="20"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19"/>
+      <c r="K106" s="19"/>
+      <c r="M106" s="19"/>
+      <c r="N106" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>